<commit_message>
changed filling akt_vh.xslx for new order (21/03/2022)
</commit_message>
<xml_diff>
--- a/Excell/akt_vh.xlsx
+++ b/Excell/akt_vh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dmitr0\Desktop\Программирование\Proj PSD\PSD\Excell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3EA0DA-87E9-48D6-B00D-6A058E3533E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AE8190-B75C-4424-AECF-AC0D40B16F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="1095" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Empty" sheetId="1" r:id="rId1"/>
@@ -898,137 +898,137 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="20% - Акцент1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1402,34 +1402,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A1" s="59"/>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
-      <c r="X1" s="59"/>
-      <c r="Y1" s="59"/>
-      <c r="Z1" s="59"/>
-      <c r="AA1" s="59"/>
-      <c r="AB1" s="59"/>
+      <c r="A1" s="80"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="80"/>
+      <c r="Q1" s="80"/>
+      <c r="R1" s="80"/>
+      <c r="S1" s="80"/>
+      <c r="T1" s="80"/>
+      <c r="U1" s="80"/>
+      <c r="V1" s="80"/>
+      <c r="W1" s="80"/>
+      <c r="X1" s="80"/>
+      <c r="Y1" s="80"/>
+      <c r="Z1" s="80"/>
+      <c r="AA1" s="80"/>
+      <c r="AB1" s="80"/>
     </row>
     <row r="2" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N2" s="3" t="s">
@@ -1437,64 +1437,64 @@
       </c>
     </row>
     <row r="3" spans="1:28" ht="2.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="68"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="68"/>
-      <c r="N3" s="68"/>
-      <c r="O3" s="68"/>
-      <c r="P3" s="68"/>
-      <c r="Q3" s="68"/>
-      <c r="R3" s="68"/>
-      <c r="S3" s="68"/>
-      <c r="T3" s="68"/>
-      <c r="U3" s="68"/>
-      <c r="V3" s="68"/>
-      <c r="W3" s="68"/>
-      <c r="X3" s="68"/>
-      <c r="Y3" s="68"/>
-      <c r="Z3" s="68"/>
-      <c r="AA3" s="68"/>
-      <c r="AB3" s="68"/>
+      <c r="A3" s="86"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="86"/>
+      <c r="R3" s="86"/>
+      <c r="S3" s="86"/>
+      <c r="T3" s="86"/>
+      <c r="U3" s="86"/>
+      <c r="V3" s="86"/>
+      <c r="W3" s="86"/>
+      <c r="X3" s="86"/>
+      <c r="Y3" s="86"/>
+      <c r="Z3" s="86"/>
+      <c r="AA3" s="86"/>
+      <c r="AB3" s="86"/>
     </row>
     <row r="4" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="69"/>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="69"/>
-      <c r="N4" s="69"/>
-      <c r="O4" s="69"/>
-      <c r="P4" s="69"/>
-      <c r="Q4" s="69"/>
-      <c r="R4" s="69"/>
-      <c r="S4" s="69"/>
-      <c r="T4" s="69"/>
-      <c r="U4" s="69"/>
-      <c r="V4" s="69"/>
-      <c r="W4" s="69"/>
-      <c r="X4" s="69"/>
-      <c r="Y4" s="69"/>
-      <c r="Z4" s="69"/>
-      <c r="AA4" s="69"/>
-      <c r="AB4" s="69"/>
+      <c r="A4" s="87"/>
+      <c r="B4" s="87"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="87"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="87"/>
+      <c r="M4" s="87"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="87"/>
+      <c r="Q4" s="87"/>
+      <c r="R4" s="87"/>
+      <c r="S4" s="87"/>
+      <c r="T4" s="87"/>
+      <c r="U4" s="87"/>
+      <c r="V4" s="87"/>
+      <c r="W4" s="87"/>
+      <c r="X4" s="87"/>
+      <c r="Y4" s="87"/>
+      <c r="Z4" s="87"/>
+      <c r="AA4" s="87"/>
+      <c r="AB4" s="87"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="N5" s="3" t="s">
@@ -1513,64 +1513,64 @@
       </c>
     </row>
     <row r="8" spans="1:28" ht="3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="70"/>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="70"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="70"/>
-      <c r="L8" s="70"/>
-      <c r="M8" s="70"/>
-      <c r="N8" s="70"/>
-      <c r="O8" s="70"/>
-      <c r="P8" s="70"/>
-      <c r="Q8" s="70"/>
-      <c r="R8" s="70"/>
-      <c r="S8" s="70"/>
-      <c r="T8" s="70"/>
-      <c r="U8" s="70"/>
-      <c r="V8" s="70"/>
-      <c r="W8" s="70"/>
-      <c r="X8" s="70"/>
-      <c r="Y8" s="70"/>
-      <c r="Z8" s="70"/>
-      <c r="AA8" s="70"/>
-      <c r="AB8" s="70"/>
+      <c r="A8" s="88"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="88"/>
+      <c r="L8" s="88"/>
+      <c r="M8" s="88"/>
+      <c r="N8" s="88"/>
+      <c r="O8" s="88"/>
+      <c r="P8" s="88"/>
+      <c r="Q8" s="88"/>
+      <c r="R8" s="88"/>
+      <c r="S8" s="88"/>
+      <c r="T8" s="88"/>
+      <c r="U8" s="88"/>
+      <c r="V8" s="88"/>
+      <c r="W8" s="88"/>
+      <c r="X8" s="88"/>
+      <c r="Y8" s="88"/>
+      <c r="Z8" s="88"/>
+      <c r="AA8" s="88"/>
+      <c r="AB8" s="88"/>
     </row>
     <row r="9" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="55"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="55"/>
-      <c r="M9" s="55"/>
-      <c r="N9" s="55"/>
-      <c r="O9" s="55"/>
-      <c r="P9" s="55"/>
-      <c r="Q9" s="55"/>
-      <c r="R9" s="55"/>
-      <c r="S9" s="55"/>
-      <c r="T9" s="55"/>
-      <c r="U9" s="55"/>
-      <c r="V9" s="55"/>
-      <c r="W9" s="55"/>
-      <c r="X9" s="55"/>
-      <c r="Y9" s="55"/>
-      <c r="Z9" s="55"/>
-      <c r="AA9" s="55"/>
-      <c r="AB9" s="55"/>
+      <c r="A9" s="89"/>
+      <c r="B9" s="89"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="89"/>
+      <c r="H9" s="89"/>
+      <c r="I9" s="89"/>
+      <c r="J9" s="89"/>
+      <c r="K9" s="89"/>
+      <c r="L9" s="89"/>
+      <c r="M9" s="89"/>
+      <c r="N9" s="89"/>
+      <c r="O9" s="89"/>
+      <c r="P9" s="89"/>
+      <c r="Q9" s="89"/>
+      <c r="R9" s="89"/>
+      <c r="S9" s="89"/>
+      <c r="T9" s="89"/>
+      <c r="U9" s="89"/>
+      <c r="V9" s="89"/>
+      <c r="W9" s="89"/>
+      <c r="X9" s="89"/>
+      <c r="Y9" s="89"/>
+      <c r="Z9" s="89"/>
+      <c r="AA9" s="89"/>
+      <c r="AB9" s="89"/>
     </row>
     <row r="10" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N10" s="7" t="s">
@@ -1656,28 +1656,28 @@
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
-      <c r="I14" s="49" t="s">
+      <c r="I14" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="50"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="50"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="50"/>
-      <c r="O14" s="50"/>
-      <c r="P14" s="50"/>
-      <c r="Q14" s="50"/>
-      <c r="R14" s="50"/>
-      <c r="S14" s="50"/>
-      <c r="T14" s="50"/>
-      <c r="U14" s="50"/>
-      <c r="V14" s="50"/>
-      <c r="W14" s="50"/>
-      <c r="X14" s="50"/>
-      <c r="Y14" s="50"/>
-      <c r="Z14" s="50"/>
-      <c r="AA14" s="50"/>
-      <c r="AB14" s="50"/>
+      <c r="J14" s="62"/>
+      <c r="K14" s="62"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="62"/>
+      <c r="N14" s="62"/>
+      <c r="O14" s="62"/>
+      <c r="P14" s="62"/>
+      <c r="Q14" s="62"/>
+      <c r="R14" s="62"/>
+      <c r="S14" s="62"/>
+      <c r="T14" s="62"/>
+      <c r="U14" s="62"/>
+      <c r="V14" s="62"/>
+      <c r="W14" s="62"/>
+      <c r="X14" s="62"/>
+      <c r="Y14" s="62"/>
+      <c r="Z14" s="62"/>
+      <c r="AA14" s="62"/>
+      <c r="AB14" s="62"/>
     </row>
     <row r="15" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
@@ -1720,40 +1720,40 @@
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
-      <c r="I16" s="49" t="s">
+      <c r="I16" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="J16" s="50"/>
-      <c r="K16" s="50"/>
-      <c r="L16" s="50"/>
-      <c r="M16" s="50"/>
-      <c r="N16" s="50"/>
-      <c r="O16" s="50"/>
-      <c r="P16" s="50"/>
-      <c r="Q16" s="50"/>
-      <c r="R16" s="50"/>
-      <c r="S16" s="50"/>
-      <c r="T16" s="50"/>
-      <c r="U16" s="50"/>
-      <c r="V16" s="50"/>
-      <c r="W16" s="50"/>
-      <c r="X16" s="50"/>
-      <c r="Y16" s="50"/>
-      <c r="Z16" s="50"/>
-      <c r="AA16" s="50"/>
-      <c r="AB16" s="50"/>
+      <c r="J16" s="62"/>
+      <c r="K16" s="62"/>
+      <c r="L16" s="62"/>
+      <c r="M16" s="62"/>
+      <c r="N16" s="62"/>
+      <c r="O16" s="62"/>
+      <c r="P16" s="62"/>
+      <c r="Q16" s="62"/>
+      <c r="R16" s="62"/>
+      <c r="S16" s="62"/>
+      <c r="T16" s="62"/>
+      <c r="U16" s="62"/>
+      <c r="V16" s="62"/>
+      <c r="W16" s="62"/>
+      <c r="X16" s="62"/>
+      <c r="Y16" s="62"/>
+      <c r="Z16" s="62"/>
+      <c r="AA16" s="62"/>
+      <c r="AB16" s="62"/>
     </row>
     <row r="17" spans="1:28" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="90" t="s">
+      <c r="A17" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="90"/>
-      <c r="C17" s="90"/>
-      <c r="D17" s="90"/>
-      <c r="E17" s="90"/>
-      <c r="F17" s="90"/>
-      <c r="G17" s="90"/>
-      <c r="H17" s="90"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
       <c r="I17" s="16"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
@@ -1782,28 +1782,28 @@
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
-      <c r="I18" s="49" t="s">
+      <c r="I18" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="50"/>
-      <c r="K18" s="50"/>
-      <c r="L18" s="50"/>
-      <c r="M18" s="50"/>
-      <c r="N18" s="50"/>
-      <c r="O18" s="50"/>
-      <c r="P18" s="50"/>
-      <c r="Q18" s="50"/>
-      <c r="R18" s="50"/>
-      <c r="S18" s="50"/>
-      <c r="T18" s="50"/>
-      <c r="U18" s="50"/>
-      <c r="V18" s="50"/>
-      <c r="W18" s="50"/>
-      <c r="X18" s="50"/>
-      <c r="Y18" s="50"/>
-      <c r="Z18" s="50"/>
-      <c r="AA18" s="50"/>
-      <c r="AB18" s="50"/>
+      <c r="J18" s="62"/>
+      <c r="K18" s="62"/>
+      <c r="L18" s="62"/>
+      <c r="M18" s="62"/>
+      <c r="N18" s="62"/>
+      <c r="O18" s="62"/>
+      <c r="P18" s="62"/>
+      <c r="Q18" s="62"/>
+      <c r="R18" s="62"/>
+      <c r="S18" s="62"/>
+      <c r="T18" s="62"/>
+      <c r="U18" s="62"/>
+      <c r="V18" s="62"/>
+      <c r="W18" s="62"/>
+      <c r="X18" s="62"/>
+      <c r="Y18" s="62"/>
+      <c r="Z18" s="62"/>
+      <c r="AA18" s="62"/>
+      <c r="AB18" s="62"/>
     </row>
     <row r="19" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
@@ -1839,45 +1839,45 @@
       <c r="F20" s="21"/>
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
-      <c r="I20" s="49" t="s">
+      <c r="I20" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="50"/>
-      <c r="K20" s="50"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="50"/>
-      <c r="O20" s="50"/>
-      <c r="P20" s="50"/>
-      <c r="Q20" s="50"/>
-      <c r="R20" s="50"/>
-      <c r="S20" s="50"/>
-      <c r="T20" s="50"/>
-      <c r="U20" s="50"/>
-      <c r="V20" s="50"/>
-      <c r="W20" s="50"/>
-      <c r="X20" s="50"/>
-      <c r="Y20" s="50"/>
-      <c r="Z20" s="50"/>
-      <c r="AA20" s="50"/>
-      <c r="AB20" s="50"/>
+      <c r="J20" s="62"/>
+      <c r="K20" s="62"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="62"/>
+      <c r="N20" s="62"/>
+      <c r="O20" s="62"/>
+      <c r="P20" s="62"/>
+      <c r="Q20" s="62"/>
+      <c r="R20" s="62"/>
+      <c r="S20" s="62"/>
+      <c r="T20" s="62"/>
+      <c r="U20" s="62"/>
+      <c r="V20" s="62"/>
+      <c r="W20" s="62"/>
+      <c r="X20" s="62"/>
+      <c r="Y20" s="62"/>
+      <c r="Z20" s="62"/>
+      <c r="AA20" s="62"/>
+      <c r="AB20" s="62"/>
     </row>
     <row r="21" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G21" s="67" t="s">
+      <c r="G21" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="53"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="53"/>
-      <c r="M21" s="53"/>
-      <c r="N21" s="53"/>
-      <c r="O21" s="53"/>
-      <c r="P21" s="53"/>
+      <c r="H21" s="60"/>
+      <c r="I21" s="60"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="60"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="60"/>
+      <c r="N21" s="60"/>
+      <c r="O21" s="60"/>
+      <c r="P21" s="60"/>
       <c r="Q21" s="2" t="s">
         <v>75</v>
       </c>
@@ -1889,18 +1889,18 @@
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
       <c r="F22" s="21"/>
-      <c r="G22" s="71" t="s">
+      <c r="G22" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="H22" s="50"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="50"/>
-      <c r="K22" s="50"/>
-      <c r="L22" s="50"/>
-      <c r="M22" s="50"/>
-      <c r="N22" s="50"/>
-      <c r="O22" s="50"/>
-      <c r="P22" s="50"/>
+      <c r="H22" s="62"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="62"/>
+      <c r="K22" s="62"/>
+      <c r="L22" s="62"/>
+      <c r="M22" s="62"/>
+      <c r="N22" s="62"/>
+      <c r="O22" s="62"/>
+      <c r="P22" s="62"/>
       <c r="Q22" s="21"/>
       <c r="R22" s="21"/>
       <c r="S22" s="21"/>
@@ -1915,37 +1915,37 @@
       <c r="AB22" s="21"/>
     </row>
     <row r="23" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="47">
+      <c r="A23" s="90">
         <f>A8</f>
         <v>0</v>
       </c>
-      <c r="B23" s="48"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="48"/>
-      <c r="K23" s="48"/>
-      <c r="L23" s="48"/>
-      <c r="M23" s="48"/>
-      <c r="N23" s="48"/>
-      <c r="O23" s="48"/>
-      <c r="P23" s="48"/>
-      <c r="Q23" s="48"/>
-      <c r="R23" s="48"/>
-      <c r="S23" s="48"/>
-      <c r="T23" s="48"/>
-      <c r="U23" s="48"/>
-      <c r="V23" s="48"/>
-      <c r="W23" s="48"/>
-      <c r="X23" s="48"/>
-      <c r="Y23" s="48"/>
-      <c r="Z23" s="48"/>
-      <c r="AA23" s="48"/>
-      <c r="AB23" s="48"/>
+      <c r="B23" s="91"/>
+      <c r="C23" s="91"/>
+      <c r="D23" s="91"/>
+      <c r="E23" s="91"/>
+      <c r="F23" s="91"/>
+      <c r="G23" s="91"/>
+      <c r="H23" s="91"/>
+      <c r="I23" s="91"/>
+      <c r="J23" s="91"/>
+      <c r="K23" s="91"/>
+      <c r="L23" s="91"/>
+      <c r="M23" s="91"/>
+      <c r="N23" s="91"/>
+      <c r="O23" s="91"/>
+      <c r="P23" s="91"/>
+      <c r="Q23" s="91"/>
+      <c r="R23" s="91"/>
+      <c r="S23" s="91"/>
+      <c r="T23" s="91"/>
+      <c r="U23" s="91"/>
+      <c r="V23" s="91"/>
+      <c r="W23" s="91"/>
+      <c r="X23" s="91"/>
+      <c r="Y23" s="91"/>
+      <c r="Z23" s="91"/>
+      <c r="AA23" s="91"/>
+      <c r="AB23" s="91"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A24" s="22"/>
@@ -1980,36 +1980,36 @@
       <c r="AB24" s="22"/>
     </row>
     <row r="25" spans="1:28" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="94" t="s">
+      <c r="A25" s="92" t="s">
         <v>90</v>
       </c>
-      <c r="B25" s="95"/>
-      <c r="C25" s="95"/>
-      <c r="D25" s="95"/>
-      <c r="E25" s="95"/>
-      <c r="F25" s="95"/>
-      <c r="G25" s="95"/>
-      <c r="H25" s="95"/>
-      <c r="I25" s="95"/>
-      <c r="J25" s="95"/>
-      <c r="K25" s="95"/>
-      <c r="L25" s="95"/>
-      <c r="M25" s="95"/>
-      <c r="N25" s="95"/>
-      <c r="O25" s="95"/>
-      <c r="P25" s="95"/>
-      <c r="Q25" s="95"/>
-      <c r="R25" s="95"/>
-      <c r="S25" s="95"/>
-      <c r="T25" s="95"/>
-      <c r="U25" s="95"/>
-      <c r="V25" s="95"/>
-      <c r="W25" s="95"/>
-      <c r="X25" s="95"/>
-      <c r="Y25" s="95"/>
-      <c r="Z25" s="95"/>
-      <c r="AA25" s="95"/>
-      <c r="AB25" s="95"/>
+      <c r="B25" s="93"/>
+      <c r="C25" s="93"/>
+      <c r="D25" s="93"/>
+      <c r="E25" s="93"/>
+      <c r="F25" s="93"/>
+      <c r="G25" s="93"/>
+      <c r="H25" s="93"/>
+      <c r="I25" s="93"/>
+      <c r="J25" s="93"/>
+      <c r="K25" s="93"/>
+      <c r="L25" s="93"/>
+      <c r="M25" s="93"/>
+      <c r="N25" s="93"/>
+      <c r="O25" s="93"/>
+      <c r="P25" s="93"/>
+      <c r="Q25" s="93"/>
+      <c r="R25" s="93"/>
+      <c r="S25" s="93"/>
+      <c r="T25" s="93"/>
+      <c r="U25" s="93"/>
+      <c r="V25" s="93"/>
+      <c r="W25" s="93"/>
+      <c r="X25" s="93"/>
+      <c r="Y25" s="93"/>
+      <c r="Z25" s="93"/>
+      <c r="AA25" s="93"/>
+      <c r="AB25" s="93"/>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A26" s="21"/>
@@ -2020,51 +2020,51 @@
       <c r="F26" s="21"/>
       <c r="G26" s="21"/>
       <c r="H26" s="21"/>
-      <c r="I26" s="56" t="s">
+      <c r="I26" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="J26" s="57"/>
-      <c r="K26" s="57"/>
-      <c r="L26" s="57"/>
-      <c r="M26" s="57"/>
-      <c r="N26" s="57"/>
-      <c r="O26" s="57"/>
-      <c r="P26" s="57"/>
-      <c r="Q26" s="57"/>
-      <c r="R26" s="57"/>
-      <c r="S26" s="57"/>
-      <c r="T26" s="57"/>
-      <c r="U26" s="57"/>
-      <c r="V26" s="57"/>
-      <c r="W26" s="57"/>
-      <c r="X26" s="57"/>
-      <c r="Y26" s="57"/>
-      <c r="Z26" s="57"/>
-      <c r="AA26" s="57"/>
-      <c r="AB26" s="57"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="54"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="54"/>
+      <c r="N26" s="54"/>
+      <c r="O26" s="54"/>
+      <c r="P26" s="54"/>
+      <c r="Q26" s="54"/>
+      <c r="R26" s="54"/>
+      <c r="S26" s="54"/>
+      <c r="T26" s="54"/>
+      <c r="U26" s="54"/>
+      <c r="V26" s="54"/>
+      <c r="W26" s="54"/>
+      <c r="X26" s="54"/>
+      <c r="Y26" s="54"/>
+      <c r="Z26" s="54"/>
+      <c r="AA26" s="54"/>
+      <c r="AB26" s="54"/>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K27" s="58"/>
-      <c r="L27" s="53"/>
-      <c r="M27" s="53"/>
-      <c r="N27" s="53"/>
-      <c r="O27" s="53"/>
-      <c r="P27" s="53"/>
-      <c r="Q27" s="53"/>
-      <c r="R27" s="53"/>
-      <c r="S27" s="53"/>
-      <c r="T27" s="53"/>
-      <c r="U27" s="53"/>
-      <c r="V27" s="53"/>
-      <c r="W27" s="53"/>
-      <c r="X27" s="53"/>
-      <c r="Y27" s="53"/>
-      <c r="Z27" s="53"/>
-      <c r="AA27" s="53"/>
-      <c r="AB27" s="53"/>
+      <c r="K27" s="68"/>
+      <c r="L27" s="60"/>
+      <c r="M27" s="60"/>
+      <c r="N27" s="60"/>
+      <c r="O27" s="60"/>
+      <c r="P27" s="60"/>
+      <c r="Q27" s="60"/>
+      <c r="R27" s="60"/>
+      <c r="S27" s="60"/>
+      <c r="T27" s="60"/>
+      <c r="U27" s="60"/>
+      <c r="V27" s="60"/>
+      <c r="W27" s="60"/>
+      <c r="X27" s="60"/>
+      <c r="Y27" s="60"/>
+      <c r="Z27" s="60"/>
+      <c r="AA27" s="60"/>
+      <c r="AB27" s="60"/>
     </row>
     <row r="28" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="21"/>
@@ -2079,24 +2079,24 @@
       <c r="J28" s="21"/>
       <c r="K28" s="21"/>
       <c r="L28" s="21"/>
-      <c r="M28" s="56" t="s">
+      <c r="M28" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="N28" s="57"/>
-      <c r="O28" s="57"/>
-      <c r="P28" s="57"/>
-      <c r="Q28" s="57"/>
-      <c r="R28" s="57"/>
-      <c r="S28" s="57"/>
-      <c r="T28" s="57"/>
-      <c r="U28" s="57"/>
-      <c r="V28" s="57"/>
-      <c r="W28" s="57"/>
-      <c r="X28" s="57"/>
-      <c r="Y28" s="57"/>
-      <c r="Z28" s="57"/>
-      <c r="AA28" s="57"/>
-      <c r="AB28" s="57"/>
+      <c r="N28" s="54"/>
+      <c r="O28" s="54"/>
+      <c r="P28" s="54"/>
+      <c r="Q28" s="54"/>
+      <c r="R28" s="54"/>
+      <c r="S28" s="54"/>
+      <c r="T28" s="54"/>
+      <c r="U28" s="54"/>
+      <c r="V28" s="54"/>
+      <c r="W28" s="54"/>
+      <c r="X28" s="54"/>
+      <c r="Y28" s="54"/>
+      <c r="Z28" s="54"/>
+      <c r="AA28" s="54"/>
+      <c r="AB28" s="54"/>
     </row>
     <row r="29" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="2" t="s">
@@ -2104,93 +2104,93 @@
       </c>
     </row>
     <row r="30" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="47">
+      <c r="A30" s="90">
         <f>A8</f>
         <v>0</v>
       </c>
-      <c r="B30" s="48"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="48"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="48"/>
-      <c r="O30" s="48"/>
-      <c r="P30" s="48"/>
-      <c r="Q30" s="48"/>
-      <c r="R30" s="48"/>
-      <c r="S30" s="48"/>
-      <c r="T30" s="48"/>
-      <c r="U30" s="48"/>
-      <c r="V30" s="48"/>
-      <c r="W30" s="48"/>
-      <c r="X30" s="48"/>
-      <c r="Y30" s="48"/>
-      <c r="Z30" s="48"/>
-      <c r="AA30" s="48"/>
-      <c r="AB30" s="48"/>
+      <c r="B30" s="91"/>
+      <c r="C30" s="91"/>
+      <c r="D30" s="91"/>
+      <c r="E30" s="91"/>
+      <c r="F30" s="91"/>
+      <c r="G30" s="91"/>
+      <c r="H30" s="91"/>
+      <c r="I30" s="91"/>
+      <c r="J30" s="91"/>
+      <c r="K30" s="91"/>
+      <c r="L30" s="91"/>
+      <c r="M30" s="91"/>
+      <c r="N30" s="91"/>
+      <c r="O30" s="91"/>
+      <c r="P30" s="91"/>
+      <c r="Q30" s="91"/>
+      <c r="R30" s="91"/>
+      <c r="S30" s="91"/>
+      <c r="T30" s="91"/>
+      <c r="U30" s="91"/>
+      <c r="V30" s="91"/>
+      <c r="W30" s="91"/>
+      <c r="X30" s="91"/>
+      <c r="Y30" s="91"/>
+      <c r="Z30" s="91"/>
+      <c r="AA30" s="91"/>
+      <c r="AB30" s="91"/>
     </row>
     <row r="31" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="50"/>
-      <c r="K31" s="50"/>
-      <c r="L31" s="50"/>
-      <c r="M31" s="50"/>
-      <c r="N31" s="50"/>
-      <c r="O31" s="50"/>
-      <c r="P31" s="50"/>
-      <c r="Q31" s="50"/>
-      <c r="R31" s="50"/>
-      <c r="S31" s="50"/>
-      <c r="T31" s="50"/>
-      <c r="U31" s="50"/>
-      <c r="V31" s="50"/>
-      <c r="W31" s="50"/>
-      <c r="X31" s="50"/>
-      <c r="Y31" s="50"/>
-      <c r="Z31" s="50"/>
-      <c r="AA31" s="50"/>
-      <c r="AB31" s="50"/>
+      <c r="B31" s="62"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="62"/>
+      <c r="F31" s="62"/>
+      <c r="G31" s="62"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="62"/>
+      <c r="J31" s="62"/>
+      <c r="K31" s="62"/>
+      <c r="L31" s="62"/>
+      <c r="M31" s="62"/>
+      <c r="N31" s="62"/>
+      <c r="O31" s="62"/>
+      <c r="P31" s="62"/>
+      <c r="Q31" s="62"/>
+      <c r="R31" s="62"/>
+      <c r="S31" s="62"/>
+      <c r="T31" s="62"/>
+      <c r="U31" s="62"/>
+      <c r="V31" s="62"/>
+      <c r="W31" s="62"/>
+      <c r="X31" s="62"/>
+      <c r="Y31" s="62"/>
+      <c r="Z31" s="62"/>
+      <c r="AA31" s="62"/>
+      <c r="AB31" s="62"/>
     </row>
     <row r="32" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J32" s="51"/>
-      <c r="K32" s="51"/>
-      <c r="L32" s="51"/>
-      <c r="M32" s="51"/>
-      <c r="N32" s="51"/>
-      <c r="O32" s="51"/>
-      <c r="P32" s="51"/>
-      <c r="Q32" s="51"/>
-      <c r="R32" s="51"/>
-      <c r="S32" s="51"/>
-      <c r="T32" s="51"/>
-      <c r="U32" s="51"/>
-      <c r="V32" s="51"/>
-      <c r="W32" s="51"/>
-      <c r="X32" s="51"/>
-      <c r="Y32" s="51"/>
-      <c r="Z32" s="51"/>
-      <c r="AA32" s="51"/>
-      <c r="AB32" s="51"/>
+      <c r="J32" s="94"/>
+      <c r="K32" s="94"/>
+      <c r="L32" s="94"/>
+      <c r="M32" s="94"/>
+      <c r="N32" s="94"/>
+      <c r="O32" s="94"/>
+      <c r="P32" s="94"/>
+      <c r="Q32" s="94"/>
+      <c r="R32" s="94"/>
+      <c r="S32" s="94"/>
+      <c r="T32" s="94"/>
+      <c r="U32" s="94"/>
+      <c r="V32" s="94"/>
+      <c r="W32" s="94"/>
+      <c r="X32" s="94"/>
+      <c r="Y32" s="94"/>
+      <c r="Z32" s="94"/>
+      <c r="AA32" s="94"/>
+      <c r="AB32" s="94"/>
     </row>
     <row r="33" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Q33" s="7" t="s">
@@ -2203,34 +2203,34 @@
       </c>
     </row>
     <row r="35" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="55"/>
-      <c r="B35" s="55"/>
-      <c r="C35" s="55"/>
-      <c r="D35" s="55"/>
-      <c r="E35" s="55"/>
-      <c r="F35" s="55"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="55"/>
-      <c r="J35" s="55"/>
-      <c r="K35" s="55"/>
-      <c r="L35" s="55"/>
-      <c r="M35" s="55"/>
-      <c r="N35" s="55"/>
-      <c r="O35" s="55"/>
-      <c r="P35" s="55"/>
-      <c r="Q35" s="55"/>
-      <c r="R35" s="55"/>
-      <c r="S35" s="55"/>
-      <c r="T35" s="55"/>
-      <c r="U35" s="55"/>
-      <c r="V35" s="55"/>
-      <c r="W35" s="55"/>
-      <c r="X35" s="55"/>
-      <c r="Y35" s="55"/>
-      <c r="Z35" s="55"/>
-      <c r="AA35" s="55"/>
-      <c r="AB35" s="55"/>
+      <c r="A35" s="89"/>
+      <c r="B35" s="89"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="89"/>
+      <c r="E35" s="89"/>
+      <c r="F35" s="89"/>
+      <c r="G35" s="89"/>
+      <c r="H35" s="89"/>
+      <c r="I35" s="89"/>
+      <c r="J35" s="89"/>
+      <c r="K35" s="89"/>
+      <c r="L35" s="89"/>
+      <c r="M35" s="89"/>
+      <c r="N35" s="89"/>
+      <c r="O35" s="89"/>
+      <c r="P35" s="89"/>
+      <c r="Q35" s="89"/>
+      <c r="R35" s="89"/>
+      <c r="S35" s="89"/>
+      <c r="T35" s="89"/>
+      <c r="U35" s="89"/>
+      <c r="V35" s="89"/>
+      <c r="W35" s="89"/>
+      <c r="X35" s="89"/>
+      <c r="Y35" s="89"/>
+      <c r="Z35" s="89"/>
+      <c r="AA35" s="89"/>
+      <c r="AB35" s="89"/>
     </row>
     <row r="36" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N36" s="7" t="s">
@@ -2412,24 +2412,24 @@
         <v>91</v>
       </c>
       <c r="K51" s="30"/>
-      <c r="L51" s="52"/>
-      <c r="M51" s="53"/>
-      <c r="N51" s="53"/>
-      <c r="O51" s="53"/>
-      <c r="P51" s="53"/>
-      <c r="Q51" s="53"/>
+      <c r="L51" s="49"/>
+      <c r="M51" s="60"/>
+      <c r="N51" s="60"/>
+      <c r="O51" s="60"/>
+      <c r="P51" s="60"/>
+      <c r="Q51" s="60"/>
       <c r="S51" s="17"/>
       <c r="T51" s="17"/>
       <c r="U51" s="17"/>
       <c r="V51" s="17"/>
       <c r="W51" s="17"/>
-      <c r="Y51" s="54">
+      <c r="Y51" s="95">
         <f>M11</f>
         <v>0</v>
       </c>
-      <c r="Z51" s="48"/>
-      <c r="AA51" s="48"/>
-      <c r="AB51" s="48"/>
+      <c r="Z51" s="91"/>
+      <c r="AA51" s="91"/>
+      <c r="AB51" s="91"/>
     </row>
     <row r="52" spans="1:28" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L52" s="21"/>
@@ -2461,24 +2461,24 @@
         <v>92</v>
       </c>
       <c r="K53" s="30"/>
-      <c r="L53" s="52"/>
-      <c r="M53" s="53"/>
-      <c r="N53" s="53"/>
-      <c r="O53" s="53"/>
-      <c r="P53" s="53"/>
-      <c r="Q53" s="53"/>
+      <c r="L53" s="49"/>
+      <c r="M53" s="60"/>
+      <c r="N53" s="60"/>
+      <c r="O53" s="60"/>
+      <c r="P53" s="60"/>
+      <c r="Q53" s="60"/>
       <c r="S53" s="17"/>
       <c r="T53" s="17"/>
       <c r="U53" s="17"/>
       <c r="V53" s="17"/>
       <c r="W53" s="17"/>
-      <c r="Y53" s="54">
+      <c r="Y53" s="95">
         <f>M11</f>
         <v>0</v>
       </c>
-      <c r="Z53" s="48"/>
-      <c r="AA53" s="48"/>
-      <c r="AB53" s="48"/>
+      <c r="Z53" s="91"/>
+      <c r="AA53" s="91"/>
+      <c r="AB53" s="91"/>
     </row>
     <row r="54" spans="1:28" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L54" s="21"/>
@@ -2506,37 +2506,37 @@
       <c r="AB54" s="21"/>
     </row>
     <row r="55" spans="1:28" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="91" t="s">
+      <c r="A55" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="B55" s="91"/>
-      <c r="C55" s="91"/>
-      <c r="D55" s="91"/>
-      <c r="E55" s="91"/>
-      <c r="F55" s="91"/>
-      <c r="G55" s="91"/>
-      <c r="H55" s="91"/>
-      <c r="I55" s="91"/>
-      <c r="J55" s="91"/>
-      <c r="K55" s="91"/>
-      <c r="L55" s="52"/>
-      <c r="M55" s="53"/>
-      <c r="N55" s="53"/>
-      <c r="O55" s="53"/>
-      <c r="P55" s="53"/>
-      <c r="Q55" s="53"/>
+      <c r="B55" s="48"/>
+      <c r="C55" s="48"/>
+      <c r="D55" s="48"/>
+      <c r="E55" s="48"/>
+      <c r="F55" s="48"/>
+      <c r="G55" s="48"/>
+      <c r="H55" s="48"/>
+      <c r="I55" s="48"/>
+      <c r="J55" s="48"/>
+      <c r="K55" s="48"/>
+      <c r="L55" s="49"/>
+      <c r="M55" s="60"/>
+      <c r="N55" s="60"/>
+      <c r="O55" s="60"/>
+      <c r="P55" s="60"/>
+      <c r="Q55" s="60"/>
       <c r="S55" s="17"/>
       <c r="T55" s="17"/>
       <c r="U55" s="17"/>
       <c r="V55" s="17"/>
       <c r="W55" s="17"/>
-      <c r="Y55" s="54">
+      <c r="Y55" s="95">
         <f>M11</f>
         <v>0</v>
       </c>
-      <c r="Z55" s="48"/>
-      <c r="AA55" s="48"/>
-      <c r="AB55" s="48"/>
+      <c r="Z55" s="91"/>
+      <c r="AA55" s="91"/>
+      <c r="AB55" s="91"/>
     </row>
     <row r="56" spans="1:28" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L56" s="21"/>
@@ -2564,37 +2564,37 @@
       <c r="AB56" s="15"/>
     </row>
     <row r="57" spans="1:28" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="91" t="s">
+      <c r="A57" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="B57" s="91"/>
-      <c r="C57" s="91"/>
-      <c r="D57" s="91"/>
-      <c r="E57" s="91"/>
-      <c r="F57" s="91"/>
-      <c r="G57" s="91"/>
-      <c r="H57" s="91"/>
-      <c r="I57" s="91"/>
-      <c r="J57" s="91"/>
-      <c r="K57" s="91"/>
-      <c r="L57" s="52"/>
-      <c r="M57" s="53"/>
-      <c r="N57" s="53"/>
-      <c r="O57" s="53"/>
-      <c r="P57" s="53"/>
-      <c r="Q57" s="53"/>
+      <c r="B57" s="48"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="48"/>
+      <c r="E57" s="48"/>
+      <c r="F57" s="48"/>
+      <c r="G57" s="48"/>
+      <c r="H57" s="48"/>
+      <c r="I57" s="48"/>
+      <c r="J57" s="48"/>
+      <c r="K57" s="48"/>
+      <c r="L57" s="49"/>
+      <c r="M57" s="60"/>
+      <c r="N57" s="60"/>
+      <c r="O57" s="60"/>
+      <c r="P57" s="60"/>
+      <c r="Q57" s="60"/>
       <c r="S57" s="17"/>
       <c r="T57" s="17"/>
       <c r="U57" s="17"/>
       <c r="V57" s="17"/>
       <c r="W57" s="17"/>
-      <c r="Y57" s="54">
+      <c r="Y57" s="95">
         <f>M11</f>
         <v>0</v>
       </c>
-      <c r="Z57" s="48"/>
-      <c r="AA57" s="48"/>
-      <c r="AB57" s="48"/>
+      <c r="Z57" s="91"/>
+      <c r="AA57" s="91"/>
+      <c r="AB57" s="91"/>
     </row>
     <row r="58" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L58" s="21"/>
@@ -2625,15 +2625,15 @@
       <c r="A59" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E59" s="60" t="s">
+      <c r="E59" s="81" t="s">
         <v>54</v>
       </c>
-      <c r="F59" s="60"/>
-      <c r="G59" s="60"/>
-      <c r="H59" s="60"/>
-      <c r="I59" s="60"/>
-      <c r="J59" s="60"/>
-      <c r="K59" s="60"/>
+      <c r="F59" s="81"/>
+      <c r="G59" s="81"/>
+      <c r="H59" s="81"/>
+      <c r="I59" s="81"/>
+      <c r="J59" s="81"/>
+      <c r="K59" s="81"/>
       <c r="AB59" s="15" t="s">
         <v>1</v>
       </c>
@@ -2642,77 +2642,77 @@
       <c r="A60" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F60" s="61" t="s">
+      <c r="F60" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="G60" s="61"/>
-      <c r="H60" s="61"/>
-      <c r="I60" s="61"/>
-      <c r="J60" s="61"/>
-      <c r="K60" s="61"/>
+      <c r="G60" s="82"/>
+      <c r="H60" s="82"/>
+      <c r="I60" s="82"/>
+      <c r="J60" s="82"/>
+      <c r="K60" s="82"/>
       <c r="S60" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="T60" s="62" t="s">
+      <c r="T60" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="U60" s="63"/>
-      <c r="V60" s="63"/>
-      <c r="W60" s="63"/>
-      <c r="X60" s="63"/>
-      <c r="Y60" s="63"/>
-      <c r="Z60" s="63"/>
-      <c r="AA60" s="63"/>
-      <c r="AB60" s="63"/>
+      <c r="U60" s="57"/>
+      <c r="V60" s="57"/>
+      <c r="W60" s="57"/>
+      <c r="X60" s="57"/>
+      <c r="Y60" s="57"/>
+      <c r="Z60" s="57"/>
+      <c r="AA60" s="57"/>
+      <c r="AB60" s="57"/>
     </row>
     <row r="61" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F61" s="17"/>
-      <c r="G61" s="64"/>
-      <c r="H61" s="64"/>
-      <c r="I61" s="64"/>
-      <c r="J61" s="64"/>
-      <c r="K61" s="64"/>
-      <c r="P61" s="65" t="s">
+      <c r="G61" s="84"/>
+      <c r="H61" s="84"/>
+      <c r="I61" s="84"/>
+      <c r="J61" s="84"/>
+      <c r="K61" s="84"/>
+      <c r="P61" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="Q61" s="65"/>
-      <c r="R61" s="65"/>
-      <c r="S61" s="65"/>
-      <c r="T61" s="66"/>
-      <c r="U61" s="66"/>
-      <c r="V61" s="66"/>
-      <c r="W61" s="66"/>
-      <c r="X61" s="66"/>
-      <c r="Y61" s="66"/>
-      <c r="Z61" s="66"/>
-      <c r="AA61" s="66"/>
-      <c r="AB61" s="66"/>
+      <c r="Q61" s="77"/>
+      <c r="R61" s="77"/>
+      <c r="S61" s="77"/>
+      <c r="T61" s="85"/>
+      <c r="U61" s="85"/>
+      <c r="V61" s="85"/>
+      <c r="W61" s="85"/>
+      <c r="X61" s="85"/>
+      <c r="Y61" s="85"/>
+      <c r="Z61" s="85"/>
+      <c r="AA61" s="85"/>
+      <c r="AB61" s="85"/>
     </row>
     <row r="62" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D62" s="67"/>
-      <c r="E62" s="67"/>
-      <c r="F62" s="67"/>
-      <c r="G62" s="67"/>
-      <c r="H62" s="67"/>
-      <c r="I62" s="67"/>
-      <c r="J62" s="67"/>
-      <c r="K62" s="67"/>
+      <c r="D62" s="59"/>
+      <c r="E62" s="59"/>
+      <c r="F62" s="59"/>
+      <c r="G62" s="59"/>
+      <c r="H62" s="59"/>
+      <c r="I62" s="59"/>
+      <c r="J62" s="59"/>
+      <c r="K62" s="59"/>
       <c r="S62" s="15"/>
-      <c r="T62" s="66"/>
-      <c r="U62" s="66"/>
-      <c r="V62" s="66"/>
-      <c r="W62" s="66"/>
-      <c r="X62" s="66"/>
-      <c r="Y62" s="66"/>
-      <c r="Z62" s="66"/>
-      <c r="AA62" s="66"/>
-      <c r="AB62" s="66"/>
+      <c r="T62" s="85"/>
+      <c r="U62" s="85"/>
+      <c r="V62" s="85"/>
+      <c r="W62" s="85"/>
+      <c r="X62" s="85"/>
+      <c r="Y62" s="85"/>
+      <c r="Z62" s="85"/>
+      <c r="AA62" s="85"/>
+      <c r="AB62" s="85"/>
     </row>
     <row r="63" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D63" s="33"/>
@@ -2725,15 +2725,15 @@
       <c r="Q63" s="34"/>
       <c r="R63" s="34"/>
       <c r="S63" s="34"/>
-      <c r="T63" s="66"/>
-      <c r="U63" s="66"/>
-      <c r="V63" s="66"/>
-      <c r="W63" s="66"/>
-      <c r="X63" s="66"/>
-      <c r="Y63" s="66"/>
-      <c r="Z63" s="66"/>
-      <c r="AA63" s="66"/>
-      <c r="AB63" s="66"/>
+      <c r="T63" s="85"/>
+      <c r="U63" s="85"/>
+      <c r="V63" s="85"/>
+      <c r="W63" s="85"/>
+      <c r="X63" s="85"/>
+      <c r="Y63" s="85"/>
+      <c r="Z63" s="85"/>
+      <c r="AA63" s="85"/>
+      <c r="AB63" s="85"/>
     </row>
     <row r="64" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D64" s="33"/>
@@ -2742,19 +2742,19 @@
       <c r="G64" s="33"/>
       <c r="H64" s="33"/>
       <c r="I64" s="33"/>
-      <c r="R64" s="72" t="s">
+      <c r="R64" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="S64" s="72"/>
-      <c r="T64" s="73"/>
-      <c r="U64" s="73"/>
-      <c r="V64" s="73"/>
-      <c r="W64" s="73"/>
-      <c r="X64" s="73"/>
-      <c r="Y64" s="73"/>
-      <c r="Z64" s="73"/>
-      <c r="AA64" s="73"/>
-      <c r="AB64" s="73"/>
+      <c r="S64" s="73"/>
+      <c r="T64" s="74"/>
+      <c r="U64" s="74"/>
+      <c r="V64" s="74"/>
+      <c r="W64" s="74"/>
+      <c r="X64" s="74"/>
+      <c r="Y64" s="74"/>
+      <c r="Z64" s="74"/>
+      <c r="AA64" s="74"/>
+      <c r="AB64" s="74"/>
     </row>
     <row r="65" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D65" s="33"/>
@@ -2766,144 +2766,144 @@
       <c r="S65" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="T65" s="74" t="s">
+      <c r="T65" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="U65" s="53"/>
-      <c r="V65" s="53"/>
-      <c r="W65" s="53"/>
-      <c r="X65" s="53"/>
-      <c r="Y65" s="53"/>
-      <c r="Z65" s="53"/>
-      <c r="AA65" s="53"/>
-      <c r="AB65" s="53"/>
+      <c r="U65" s="60"/>
+      <c r="V65" s="60"/>
+      <c r="W65" s="60"/>
+      <c r="X65" s="60"/>
+      <c r="Y65" s="60"/>
+      <c r="Z65" s="60"/>
+      <c r="AA65" s="60"/>
+      <c r="AB65" s="60"/>
     </row>
     <row r="66" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="Q66" s="75" t="s">
+      <c r="Q66" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="R66" s="53"/>
-      <c r="S66" s="53"/>
-      <c r="T66" s="53"/>
-      <c r="U66" s="53"/>
-      <c r="V66" s="53"/>
-      <c r="W66" s="53"/>
-      <c r="X66" s="53"/>
-      <c r="Y66" s="53"/>
-      <c r="Z66" s="53"/>
-      <c r="AA66" s="53"/>
-      <c r="AB66" s="53"/>
+      <c r="R66" s="60"/>
+      <c r="S66" s="60"/>
+      <c r="T66" s="60"/>
+      <c r="U66" s="60"/>
+      <c r="V66" s="60"/>
+      <c r="W66" s="60"/>
+      <c r="X66" s="60"/>
+      <c r="Y66" s="60"/>
+      <c r="Z66" s="60"/>
+      <c r="AA66" s="60"/>
+      <c r="AB66" s="60"/>
     </row>
     <row r="67" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="M67" s="65" t="s">
+      <c r="M67" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="N67" s="76"/>
-      <c r="O67" s="76"/>
+      <c r="N67" s="71"/>
+      <c r="O67" s="71"/>
       <c r="P67" s="35"/>
       <c r="V67" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="W67" s="77"/>
-      <c r="X67" s="78"/>
-      <c r="Y67" s="78"/>
-      <c r="Z67" s="78"/>
-      <c r="AA67" s="78"/>
-      <c r="AB67" s="78"/>
+      <c r="W67" s="78"/>
+      <c r="X67" s="79"/>
+      <c r="Y67" s="79"/>
+      <c r="Z67" s="79"/>
+      <c r="AA67" s="79"/>
+      <c r="AB67" s="79"/>
     </row>
     <row r="68" spans="1:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="79" t="s">
+      <c r="A68" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="B68" s="76"/>
-      <c r="C68" s="76"/>
-      <c r="D68" s="76"/>
-      <c r="E68" s="76"/>
-      <c r="F68" s="76"/>
-      <c r="G68" s="76"/>
-      <c r="H68" s="76"/>
-      <c r="I68" s="76"/>
-      <c r="J68" s="76"/>
-      <c r="K68" s="76"/>
-      <c r="L68" s="76"/>
-      <c r="M68" s="76"/>
-      <c r="N68" s="76"/>
-      <c r="O68" s="76"/>
-      <c r="P68" s="76"/>
-      <c r="Q68" s="76"/>
-      <c r="R68" s="76"/>
-      <c r="S68" s="76"/>
-      <c r="T68" s="76"/>
-      <c r="U68" s="76"/>
-      <c r="V68" s="76"/>
-      <c r="W68" s="76"/>
-      <c r="X68" s="76"/>
-      <c r="Y68" s="76"/>
-      <c r="Z68" s="76"/>
-      <c r="AA68" s="76"/>
-      <c r="AB68" s="76"/>
+      <c r="B68" s="71"/>
+      <c r="C68" s="71"/>
+      <c r="D68" s="71"/>
+      <c r="E68" s="71"/>
+      <c r="F68" s="71"/>
+      <c r="G68" s="71"/>
+      <c r="H68" s="71"/>
+      <c r="I68" s="71"/>
+      <c r="J68" s="71"/>
+      <c r="K68" s="71"/>
+      <c r="L68" s="71"/>
+      <c r="M68" s="71"/>
+      <c r="N68" s="71"/>
+      <c r="O68" s="71"/>
+      <c r="P68" s="71"/>
+      <c r="Q68" s="71"/>
+      <c r="R68" s="71"/>
+      <c r="S68" s="71"/>
+      <c r="T68" s="71"/>
+      <c r="U68" s="71"/>
+      <c r="V68" s="71"/>
+      <c r="W68" s="71"/>
+      <c r="X68" s="71"/>
+      <c r="Y68" s="71"/>
+      <c r="Z68" s="71"/>
+      <c r="AA68" s="71"/>
+      <c r="AB68" s="71"/>
     </row>
     <row r="69" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A69" s="13"/>
-      <c r="B69" s="80"/>
-      <c r="C69" s="81"/>
-      <c r="D69" s="81"/>
-      <c r="E69" s="81"/>
-      <c r="F69" s="81"/>
-      <c r="G69" s="81"/>
-      <c r="H69" s="81"/>
-      <c r="I69" s="81"/>
-      <c r="J69" s="81"/>
-      <c r="K69" s="81"/>
-      <c r="L69" s="81"/>
-      <c r="M69" s="81"/>
-      <c r="N69" s="81"/>
-      <c r="O69" s="81"/>
-      <c r="P69" s="81"/>
-      <c r="Q69" s="81"/>
-      <c r="R69" s="81"/>
-      <c r="S69" s="81"/>
-      <c r="T69" s="81"/>
-      <c r="U69" s="81"/>
-      <c r="V69" s="81"/>
-      <c r="W69" s="81"/>
-      <c r="X69" s="81"/>
-      <c r="Y69" s="81"/>
-      <c r="Z69" s="81"/>
-      <c r="AA69" s="81"/>
+      <c r="B69" s="63"/>
+      <c r="C69" s="51"/>
+      <c r="D69" s="51"/>
+      <c r="E69" s="51"/>
+      <c r="F69" s="51"/>
+      <c r="G69" s="51"/>
+      <c r="H69" s="51"/>
+      <c r="I69" s="51"/>
+      <c r="J69" s="51"/>
+      <c r="K69" s="51"/>
+      <c r="L69" s="51"/>
+      <c r="M69" s="51"/>
+      <c r="N69" s="51"/>
+      <c r="O69" s="51"/>
+      <c r="P69" s="51"/>
+      <c r="Q69" s="51"/>
+      <c r="R69" s="51"/>
+      <c r="S69" s="51"/>
+      <c r="T69" s="51"/>
+      <c r="U69" s="51"/>
+      <c r="V69" s="51"/>
+      <c r="W69" s="51"/>
+      <c r="X69" s="51"/>
+      <c r="Y69" s="51"/>
+      <c r="Z69" s="51"/>
+      <c r="AA69" s="51"/>
       <c r="AB69" s="13"/>
     </row>
     <row r="70" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A70" s="82" t="s">
+      <c r="A70" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="B70" s="50"/>
-      <c r="C70" s="50"/>
-      <c r="D70" s="50"/>
-      <c r="E70" s="50"/>
-      <c r="F70" s="50"/>
-      <c r="G70" s="50"/>
-      <c r="H70" s="50"/>
-      <c r="I70" s="50"/>
-      <c r="J70" s="50"/>
-      <c r="K70" s="50"/>
-      <c r="L70" s="50"/>
-      <c r="M70" s="50"/>
-      <c r="N70" s="50"/>
-      <c r="O70" s="50"/>
-      <c r="P70" s="50"/>
-      <c r="Q70" s="50"/>
-      <c r="R70" s="50"/>
-      <c r="S70" s="50"/>
-      <c r="T70" s="50"/>
-      <c r="U70" s="50"/>
-      <c r="V70" s="50"/>
-      <c r="W70" s="50"/>
-      <c r="X70" s="50"/>
-      <c r="Y70" s="50"/>
-      <c r="Z70" s="50"/>
-      <c r="AA70" s="50"/>
-      <c r="AB70" s="50"/>
+      <c r="B70" s="62"/>
+      <c r="C70" s="62"/>
+      <c r="D70" s="62"/>
+      <c r="E70" s="62"/>
+      <c r="F70" s="62"/>
+      <c r="G70" s="62"/>
+      <c r="H70" s="62"/>
+      <c r="I70" s="62"/>
+      <c r="J70" s="62"/>
+      <c r="K70" s="62"/>
+      <c r="L70" s="62"/>
+      <c r="M70" s="62"/>
+      <c r="N70" s="62"/>
+      <c r="O70" s="62"/>
+      <c r="P70" s="62"/>
+      <c r="Q70" s="62"/>
+      <c r="R70" s="62"/>
+      <c r="S70" s="62"/>
+      <c r="T70" s="62"/>
+      <c r="U70" s="62"/>
+      <c r="V70" s="62"/>
+      <c r="W70" s="62"/>
+      <c r="X70" s="62"/>
+      <c r="Y70" s="62"/>
+      <c r="Z70" s="62"/>
+      <c r="AA70" s="62"/>
+      <c r="AB70" s="62"/>
     </row>
     <row r="71" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A71" s="9"/>
@@ -2963,28 +2963,28 @@
       <c r="AB72" s="13"/>
     </row>
     <row r="73" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="I73" s="49" t="s">
+      <c r="I73" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="J73" s="50"/>
-      <c r="K73" s="50"/>
-      <c r="L73" s="50"/>
-      <c r="M73" s="50"/>
-      <c r="N73" s="50"/>
-      <c r="O73" s="50"/>
-      <c r="P73" s="50"/>
-      <c r="Q73" s="50"/>
-      <c r="R73" s="50"/>
-      <c r="S73" s="50"/>
-      <c r="T73" s="50"/>
-      <c r="U73" s="50"/>
-      <c r="V73" s="50"/>
-      <c r="W73" s="50"/>
-      <c r="X73" s="50"/>
-      <c r="Y73" s="50"/>
-      <c r="Z73" s="50"/>
-      <c r="AA73" s="50"/>
-      <c r="AB73" s="50"/>
+      <c r="J73" s="62"/>
+      <c r="K73" s="62"/>
+      <c r="L73" s="62"/>
+      <c r="M73" s="62"/>
+      <c r="N73" s="62"/>
+      <c r="O73" s="62"/>
+      <c r="P73" s="62"/>
+      <c r="Q73" s="62"/>
+      <c r="R73" s="62"/>
+      <c r="S73" s="62"/>
+      <c r="T73" s="62"/>
+      <c r="U73" s="62"/>
+      <c r="V73" s="62"/>
+      <c r="W73" s="62"/>
+      <c r="X73" s="62"/>
+      <c r="Y73" s="62"/>
+      <c r="Z73" s="62"/>
+      <c r="AA73" s="62"/>
+      <c r="AB73" s="62"/>
     </row>
     <row r="74" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
@@ -3013,28 +3013,28 @@
       <c r="AB74" s="13"/>
     </row>
     <row r="75" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="I75" s="49" t="s">
+      <c r="I75" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="J75" s="50"/>
-      <c r="K75" s="50"/>
-      <c r="L75" s="50"/>
-      <c r="M75" s="50"/>
-      <c r="N75" s="50"/>
-      <c r="O75" s="50"/>
-      <c r="P75" s="50"/>
-      <c r="Q75" s="50"/>
-      <c r="R75" s="50"/>
-      <c r="S75" s="50"/>
-      <c r="T75" s="50"/>
-      <c r="U75" s="50"/>
-      <c r="V75" s="50"/>
-      <c r="W75" s="50"/>
-      <c r="X75" s="50"/>
-      <c r="Y75" s="50"/>
-      <c r="Z75" s="50"/>
-      <c r="AA75" s="50"/>
-      <c r="AB75" s="50"/>
+      <c r="J75" s="62"/>
+      <c r="K75" s="62"/>
+      <c r="L75" s="62"/>
+      <c r="M75" s="62"/>
+      <c r="N75" s="62"/>
+      <c r="O75" s="62"/>
+      <c r="P75" s="62"/>
+      <c r="Q75" s="62"/>
+      <c r="R75" s="62"/>
+      <c r="S75" s="62"/>
+      <c r="T75" s="62"/>
+      <c r="U75" s="62"/>
+      <c r="V75" s="62"/>
+      <c r="W75" s="62"/>
+      <c r="X75" s="62"/>
+      <c r="Y75" s="62"/>
+      <c r="Z75" s="62"/>
+      <c r="AA75" s="62"/>
+      <c r="AB75" s="62"/>
     </row>
     <row r="76" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
@@ -3066,28 +3066,28 @@
       <c r="F77" s="21"/>
       <c r="G77" s="21"/>
       <c r="H77" s="21"/>
-      <c r="I77" s="49" t="s">
+      <c r="I77" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="J77" s="50"/>
-      <c r="K77" s="50"/>
-      <c r="L77" s="50"/>
-      <c r="M77" s="50"/>
-      <c r="N77" s="50"/>
-      <c r="O77" s="50"/>
-      <c r="P77" s="50"/>
-      <c r="Q77" s="50"/>
-      <c r="R77" s="50"/>
-      <c r="S77" s="50"/>
-      <c r="T77" s="50"/>
-      <c r="U77" s="50"/>
-      <c r="V77" s="50"/>
-      <c r="W77" s="50"/>
-      <c r="X77" s="50"/>
-      <c r="Y77" s="50"/>
-      <c r="Z77" s="50"/>
-      <c r="AA77" s="50"/>
-      <c r="AB77" s="50"/>
+      <c r="J77" s="62"/>
+      <c r="K77" s="62"/>
+      <c r="L77" s="62"/>
+      <c r="M77" s="62"/>
+      <c r="N77" s="62"/>
+      <c r="O77" s="62"/>
+      <c r="P77" s="62"/>
+      <c r="Q77" s="62"/>
+      <c r="R77" s="62"/>
+      <c r="S77" s="62"/>
+      <c r="T77" s="62"/>
+      <c r="U77" s="62"/>
+      <c r="V77" s="62"/>
+      <c r="W77" s="62"/>
+      <c r="X77" s="62"/>
+      <c r="Y77" s="62"/>
+      <c r="Z77" s="62"/>
+      <c r="AA77" s="62"/>
+      <c r="AB77" s="62"/>
     </row>
     <row r="78" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
@@ -3129,28 +3129,28 @@
       <c r="F79" s="21"/>
       <c r="G79" s="21"/>
       <c r="H79" s="21"/>
-      <c r="I79" s="49" t="s">
+      <c r="I79" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="J79" s="50"/>
-      <c r="K79" s="50"/>
-      <c r="L79" s="50"/>
-      <c r="M79" s="50"/>
-      <c r="N79" s="50"/>
-      <c r="O79" s="50"/>
-      <c r="P79" s="50"/>
-      <c r="Q79" s="50"/>
-      <c r="R79" s="50"/>
-      <c r="S79" s="50"/>
-      <c r="T79" s="50"/>
-      <c r="U79" s="50"/>
-      <c r="V79" s="50"/>
-      <c r="W79" s="50"/>
-      <c r="X79" s="50"/>
-      <c r="Y79" s="50"/>
-      <c r="Z79" s="50"/>
-      <c r="AA79" s="50"/>
-      <c r="AB79" s="50"/>
+      <c r="J79" s="62"/>
+      <c r="K79" s="62"/>
+      <c r="L79" s="62"/>
+      <c r="M79" s="62"/>
+      <c r="N79" s="62"/>
+      <c r="O79" s="62"/>
+      <c r="P79" s="62"/>
+      <c r="Q79" s="62"/>
+      <c r="R79" s="62"/>
+      <c r="S79" s="62"/>
+      <c r="T79" s="62"/>
+      <c r="U79" s="62"/>
+      <c r="V79" s="62"/>
+      <c r="W79" s="62"/>
+      <c r="X79" s="62"/>
+      <c r="Y79" s="62"/>
+      <c r="Z79" s="62"/>
+      <c r="AA79" s="62"/>
+      <c r="AB79" s="62"/>
     </row>
     <row r="80" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
@@ -3182,45 +3182,45 @@
       <c r="F81" s="21"/>
       <c r="G81" s="21"/>
       <c r="H81" s="21"/>
-      <c r="I81" s="49" t="s">
+      <c r="I81" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="J81" s="50"/>
-      <c r="K81" s="50"/>
-      <c r="L81" s="50"/>
-      <c r="M81" s="50"/>
-      <c r="N81" s="50"/>
-      <c r="O81" s="50"/>
-      <c r="P81" s="50"/>
-      <c r="Q81" s="50"/>
-      <c r="R81" s="50"/>
-      <c r="S81" s="50"/>
-      <c r="T81" s="50"/>
-      <c r="U81" s="50"/>
-      <c r="V81" s="50"/>
-      <c r="W81" s="50"/>
-      <c r="X81" s="50"/>
-      <c r="Y81" s="50"/>
-      <c r="Z81" s="50"/>
-      <c r="AA81" s="50"/>
-      <c r="AB81" s="50"/>
+      <c r="J81" s="62"/>
+      <c r="K81" s="62"/>
+      <c r="L81" s="62"/>
+      <c r="M81" s="62"/>
+      <c r="N81" s="62"/>
+      <c r="O81" s="62"/>
+      <c r="P81" s="62"/>
+      <c r="Q81" s="62"/>
+      <c r="R81" s="62"/>
+      <c r="S81" s="62"/>
+      <c r="T81" s="62"/>
+      <c r="U81" s="62"/>
+      <c r="V81" s="62"/>
+      <c r="W81" s="62"/>
+      <c r="X81" s="62"/>
+      <c r="Y81" s="62"/>
+      <c r="Z81" s="62"/>
+      <c r="AA81" s="62"/>
+      <c r="AB81" s="62"/>
     </row>
     <row r="82" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G82" s="67" t="s">
+      <c r="G82" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="H82" s="53"/>
-      <c r="I82" s="53"/>
-      <c r="J82" s="53"/>
-      <c r="K82" s="53"/>
-      <c r="L82" s="53"/>
-      <c r="M82" s="53"/>
-      <c r="N82" s="53"/>
-      <c r="O82" s="53"/>
-      <c r="P82" s="53"/>
+      <c r="H82" s="60"/>
+      <c r="I82" s="60"/>
+      <c r="J82" s="60"/>
+      <c r="K82" s="60"/>
+      <c r="L82" s="60"/>
+      <c r="M82" s="60"/>
+      <c r="N82" s="60"/>
+      <c r="O82" s="60"/>
+      <c r="P82" s="60"/>
       <c r="Q82" s="2" t="s">
         <v>26</v>
       </c>
@@ -3232,18 +3232,18 @@
       <c r="D83" s="21"/>
       <c r="E83" s="21"/>
       <c r="F83" s="21"/>
-      <c r="G83" s="71" t="s">
+      <c r="G83" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="H83" s="50"/>
-      <c r="I83" s="50"/>
-      <c r="J83" s="50"/>
-      <c r="K83" s="50"/>
-      <c r="L83" s="50"/>
-      <c r="M83" s="50"/>
-      <c r="N83" s="50"/>
-      <c r="O83" s="50"/>
-      <c r="P83" s="50"/>
+      <c r="H83" s="62"/>
+      <c r="I83" s="62"/>
+      <c r="J83" s="62"/>
+      <c r="K83" s="62"/>
+      <c r="L83" s="62"/>
+      <c r="M83" s="62"/>
+      <c r="N83" s="62"/>
+      <c r="O83" s="62"/>
+      <c r="P83" s="62"/>
       <c r="Q83" s="21"/>
       <c r="R83" s="21"/>
       <c r="S83" s="21"/>
@@ -3258,37 +3258,37 @@
       <c r="AB83" s="21"/>
     </row>
     <row r="84" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A84" s="80">
+      <c r="A84" s="63">
         <f>B69</f>
         <v>0</v>
       </c>
-      <c r="B84" s="80"/>
-      <c r="C84" s="80"/>
-      <c r="D84" s="80"/>
-      <c r="E84" s="80"/>
-      <c r="F84" s="80"/>
-      <c r="G84" s="80"/>
-      <c r="H84" s="80"/>
-      <c r="I84" s="80"/>
-      <c r="J84" s="80"/>
-      <c r="K84" s="80"/>
-      <c r="L84" s="80"/>
-      <c r="M84" s="80"/>
-      <c r="N84" s="80"/>
-      <c r="O84" s="80"/>
-      <c r="P84" s="80"/>
-      <c r="Q84" s="80"/>
-      <c r="R84" s="80"/>
-      <c r="S84" s="80"/>
-      <c r="T84" s="80"/>
-      <c r="U84" s="80"/>
-      <c r="V84" s="80"/>
-      <c r="W84" s="80"/>
-      <c r="X84" s="80"/>
-      <c r="Y84" s="80"/>
-      <c r="Z84" s="80"/>
-      <c r="AA84" s="80"/>
-      <c r="AB84" s="80"/>
+      <c r="B84" s="63"/>
+      <c r="C84" s="63"/>
+      <c r="D84" s="63"/>
+      <c r="E84" s="63"/>
+      <c r="F84" s="63"/>
+      <c r="G84" s="63"/>
+      <c r="H84" s="63"/>
+      <c r="I84" s="63"/>
+      <c r="J84" s="63"/>
+      <c r="K84" s="63"/>
+      <c r="L84" s="63"/>
+      <c r="M84" s="63"/>
+      <c r="N84" s="63"/>
+      <c r="O84" s="63"/>
+      <c r="P84" s="63"/>
+      <c r="Q84" s="63"/>
+      <c r="R84" s="63"/>
+      <c r="S84" s="63"/>
+      <c r="T84" s="63"/>
+      <c r="U84" s="63"/>
+      <c r="V84" s="63"/>
+      <c r="W84" s="63"/>
+      <c r="X84" s="63"/>
+      <c r="Y84" s="63"/>
+      <c r="Z84" s="63"/>
+      <c r="AA84" s="63"/>
+      <c r="AB84" s="63"/>
     </row>
     <row r="85" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A85" s="22"/>
@@ -3323,36 +3323,36 @@
       <c r="AB85" s="22"/>
     </row>
     <row r="86" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A86" s="83" t="s">
+      <c r="A86" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="B86" s="83"/>
-      <c r="C86" s="83"/>
-      <c r="D86" s="83"/>
-      <c r="E86" s="83"/>
-      <c r="F86" s="83"/>
-      <c r="G86" s="83"/>
-      <c r="H86" s="83"/>
-      <c r="I86" s="83"/>
-      <c r="J86" s="83"/>
-      <c r="K86" s="83"/>
-      <c r="L86" s="83"/>
-      <c r="M86" s="83"/>
-      <c r="N86" s="83"/>
-      <c r="O86" s="83"/>
-      <c r="P86" s="83"/>
-      <c r="Q86" s="83"/>
-      <c r="R86" s="83"/>
-      <c r="S86" s="83"/>
-      <c r="T86" s="83"/>
-      <c r="U86" s="83"/>
-      <c r="V86" s="83"/>
-      <c r="W86" s="83"/>
-      <c r="X86" s="83"/>
-      <c r="Y86" s="83"/>
-      <c r="Z86" s="83"/>
-      <c r="AA86" s="83"/>
-      <c r="AB86" s="83"/>
+      <c r="B86" s="67"/>
+      <c r="C86" s="67"/>
+      <c r="D86" s="67"/>
+      <c r="E86" s="67"/>
+      <c r="F86" s="67"/>
+      <c r="G86" s="67"/>
+      <c r="H86" s="67"/>
+      <c r="I86" s="67"/>
+      <c r="J86" s="67"/>
+      <c r="K86" s="67"/>
+      <c r="L86" s="67"/>
+      <c r="M86" s="67"/>
+      <c r="N86" s="67"/>
+      <c r="O86" s="67"/>
+      <c r="P86" s="67"/>
+      <c r="Q86" s="67"/>
+      <c r="R86" s="67"/>
+      <c r="S86" s="67"/>
+      <c r="T86" s="67"/>
+      <c r="U86" s="67"/>
+      <c r="V86" s="67"/>
+      <c r="W86" s="67"/>
+      <c r="X86" s="67"/>
+      <c r="Y86" s="67"/>
+      <c r="Z86" s="67"/>
+      <c r="AA86" s="67"/>
+      <c r="AB86" s="67"/>
     </row>
     <row r="87" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A87" s="21"/>
@@ -3363,54 +3363,54 @@
       <c r="F87" s="21"/>
       <c r="G87" s="21"/>
       <c r="H87" s="21"/>
-      <c r="I87" s="56" t="s">
+      <c r="I87" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="J87" s="57"/>
-      <c r="K87" s="57"/>
-      <c r="L87" s="57"/>
-      <c r="M87" s="57"/>
-      <c r="N87" s="57"/>
-      <c r="O87" s="57"/>
-      <c r="P87" s="57"/>
-      <c r="Q87" s="57"/>
-      <c r="R87" s="57"/>
-      <c r="S87" s="57"/>
-      <c r="T87" s="57"/>
-      <c r="U87" s="57"/>
-      <c r="V87" s="57"/>
-      <c r="W87" s="57"/>
-      <c r="X87" s="57"/>
-      <c r="Y87" s="57"/>
-      <c r="Z87" s="57"/>
-      <c r="AA87" s="57"/>
-      <c r="AB87" s="57"/>
+      <c r="J87" s="54"/>
+      <c r="K87" s="54"/>
+      <c r="L87" s="54"/>
+      <c r="M87" s="54"/>
+      <c r="N87" s="54"/>
+      <c r="O87" s="54"/>
+      <c r="P87" s="54"/>
+      <c r="Q87" s="54"/>
+      <c r="R87" s="54"/>
+      <c r="S87" s="54"/>
+      <c r="T87" s="54"/>
+      <c r="U87" s="54"/>
+      <c r="V87" s="54"/>
+      <c r="W87" s="54"/>
+      <c r="X87" s="54"/>
+      <c r="Y87" s="54"/>
+      <c r="Z87" s="54"/>
+      <c r="AA87" s="54"/>
+      <c r="AB87" s="54"/>
     </row>
     <row r="88" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A88" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="K88" s="58">
+      <c r="K88" s="68">
         <f>T64</f>
         <v>0</v>
       </c>
-      <c r="L88" s="58"/>
-      <c r="M88" s="58"/>
-      <c r="N88" s="58"/>
-      <c r="O88" s="58"/>
-      <c r="P88" s="58"/>
-      <c r="Q88" s="58"/>
-      <c r="R88" s="58"/>
-      <c r="S88" s="58"/>
-      <c r="T88" s="58"/>
-      <c r="U88" s="58"/>
-      <c r="V88" s="58"/>
-      <c r="W88" s="58"/>
-      <c r="X88" s="58"/>
-      <c r="Y88" s="58"/>
-      <c r="Z88" s="58"/>
-      <c r="AA88" s="58"/>
-      <c r="AB88" s="58"/>
+      <c r="L88" s="68"/>
+      <c r="M88" s="68"/>
+      <c r="N88" s="68"/>
+      <c r="O88" s="68"/>
+      <c r="P88" s="68"/>
+      <c r="Q88" s="68"/>
+      <c r="R88" s="68"/>
+      <c r="S88" s="68"/>
+      <c r="T88" s="68"/>
+      <c r="U88" s="68"/>
+      <c r="V88" s="68"/>
+      <c r="W88" s="68"/>
+      <c r="X88" s="68"/>
+      <c r="Y88" s="68"/>
+      <c r="Z88" s="68"/>
+      <c r="AA88" s="68"/>
+      <c r="AB88" s="68"/>
     </row>
     <row r="89" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A89" s="21"/>
@@ -3425,24 +3425,24 @@
       <c r="J89" s="21"/>
       <c r="K89" s="21"/>
       <c r="L89" s="21"/>
-      <c r="M89" s="56" t="s">
+      <c r="M89" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="N89" s="57"/>
-      <c r="O89" s="57"/>
-      <c r="P89" s="57"/>
-      <c r="Q89" s="57"/>
-      <c r="R89" s="57"/>
-      <c r="S89" s="57"/>
-      <c r="T89" s="57"/>
-      <c r="U89" s="57"/>
-      <c r="V89" s="57"/>
-      <c r="W89" s="57"/>
-      <c r="X89" s="57"/>
-      <c r="Y89" s="57"/>
-      <c r="Z89" s="57"/>
-      <c r="AA89" s="57"/>
-      <c r="AB89" s="57"/>
+      <c r="N89" s="54"/>
+      <c r="O89" s="54"/>
+      <c r="P89" s="54"/>
+      <c r="Q89" s="54"/>
+      <c r="R89" s="54"/>
+      <c r="S89" s="54"/>
+      <c r="T89" s="54"/>
+      <c r="U89" s="54"/>
+      <c r="V89" s="54"/>
+      <c r="W89" s="54"/>
+      <c r="X89" s="54"/>
+      <c r="Y89" s="54"/>
+      <c r="Z89" s="54"/>
+      <c r="AA89" s="54"/>
+      <c r="AB89" s="54"/>
     </row>
     <row r="90" spans="1:28" x14ac:dyDescent="0.3">
       <c r="C90" s="2" t="s">
@@ -3450,69 +3450,69 @@
       </c>
     </row>
     <row r="91" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A91" s="80">
+      <c r="A91" s="63">
         <f>B69</f>
         <v>0</v>
       </c>
-      <c r="B91" s="80"/>
-      <c r="C91" s="80"/>
-      <c r="D91" s="80"/>
-      <c r="E91" s="80"/>
-      <c r="F91" s="80"/>
-      <c r="G91" s="80"/>
-      <c r="H91" s="80"/>
-      <c r="I91" s="80"/>
-      <c r="J91" s="80"/>
-      <c r="K91" s="80"/>
-      <c r="L91" s="80"/>
-      <c r="M91" s="80"/>
-      <c r="N91" s="80"/>
-      <c r="O91" s="80"/>
-      <c r="P91" s="80"/>
-      <c r="Q91" s="80"/>
-      <c r="R91" s="80"/>
-      <c r="S91" s="80"/>
-      <c r="T91" s="80"/>
-      <c r="U91" s="80"/>
-      <c r="V91" s="80"/>
-      <c r="W91" s="80"/>
-      <c r="X91" s="80"/>
-      <c r="Y91" s="80"/>
-      <c r="Z91" s="80"/>
-      <c r="AA91" s="80"/>
-      <c r="AB91" s="80"/>
+      <c r="B91" s="63"/>
+      <c r="C91" s="63"/>
+      <c r="D91" s="63"/>
+      <c r="E91" s="63"/>
+      <c r="F91" s="63"/>
+      <c r="G91" s="63"/>
+      <c r="H91" s="63"/>
+      <c r="I91" s="63"/>
+      <c r="J91" s="63"/>
+      <c r="K91" s="63"/>
+      <c r="L91" s="63"/>
+      <c r="M91" s="63"/>
+      <c r="N91" s="63"/>
+      <c r="O91" s="63"/>
+      <c r="P91" s="63"/>
+      <c r="Q91" s="63"/>
+      <c r="R91" s="63"/>
+      <c r="S91" s="63"/>
+      <c r="T91" s="63"/>
+      <c r="U91" s="63"/>
+      <c r="V91" s="63"/>
+      <c r="W91" s="63"/>
+      <c r="X91" s="63"/>
+      <c r="Y91" s="63"/>
+      <c r="Z91" s="63"/>
+      <c r="AA91" s="63"/>
+      <c r="AB91" s="63"/>
     </row>
     <row r="92" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A92" s="49" t="s">
+      <c r="A92" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="B92" s="50"/>
-      <c r="C92" s="50"/>
-      <c r="D92" s="50"/>
-      <c r="E92" s="50"/>
-      <c r="F92" s="50"/>
-      <c r="G92" s="50"/>
-      <c r="H92" s="50"/>
-      <c r="I92" s="50"/>
-      <c r="J92" s="50"/>
-      <c r="K92" s="50"/>
-      <c r="L92" s="50"/>
-      <c r="M92" s="50"/>
-      <c r="N92" s="50"/>
-      <c r="O92" s="50"/>
-      <c r="P92" s="50"/>
-      <c r="Q92" s="50"/>
-      <c r="R92" s="50"/>
-      <c r="S92" s="50"/>
-      <c r="T92" s="50"/>
-      <c r="U92" s="50"/>
-      <c r="V92" s="50"/>
-      <c r="W92" s="50"/>
-      <c r="X92" s="50"/>
-      <c r="Y92" s="50"/>
-      <c r="Z92" s="50"/>
-      <c r="AA92" s="50"/>
-      <c r="AB92" s="50"/>
+      <c r="B92" s="62"/>
+      <c r="C92" s="62"/>
+      <c r="D92" s="62"/>
+      <c r="E92" s="62"/>
+      <c r="F92" s="62"/>
+      <c r="G92" s="62"/>
+      <c r="H92" s="62"/>
+      <c r="I92" s="62"/>
+      <c r="J92" s="62"/>
+      <c r="K92" s="62"/>
+      <c r="L92" s="62"/>
+      <c r="M92" s="62"/>
+      <c r="N92" s="62"/>
+      <c r="O92" s="62"/>
+      <c r="P92" s="62"/>
+      <c r="Q92" s="62"/>
+      <c r="R92" s="62"/>
+      <c r="S92" s="62"/>
+      <c r="T92" s="62"/>
+      <c r="U92" s="62"/>
+      <c r="V92" s="62"/>
+      <c r="W92" s="62"/>
+      <c r="X92" s="62"/>
+      <c r="Y92" s="62"/>
+      <c r="Z92" s="62"/>
+      <c r="AA92" s="62"/>
+      <c r="AB92" s="62"/>
     </row>
     <row r="93" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A93" s="39" t="s">
@@ -3529,22 +3529,22 @@
       <c r="J93" s="40"/>
       <c r="K93" s="40"/>
       <c r="L93" s="40"/>
-      <c r="M93" s="84"/>
-      <c r="N93" s="84"/>
-      <c r="O93" s="84"/>
-      <c r="P93" s="84"/>
-      <c r="Q93" s="84"/>
-      <c r="R93" s="84"/>
-      <c r="S93" s="84"/>
-      <c r="T93" s="84"/>
-      <c r="U93" s="84"/>
-      <c r="V93" s="84"/>
-      <c r="W93" s="84"/>
-      <c r="X93" s="84"/>
-      <c r="Y93" s="84"/>
-      <c r="Z93" s="84"/>
-      <c r="AA93" s="84"/>
-      <c r="AB93" s="84"/>
+      <c r="M93" s="65"/>
+      <c r="N93" s="65"/>
+      <c r="O93" s="65"/>
+      <c r="P93" s="65"/>
+      <c r="Q93" s="65"/>
+      <c r="R93" s="65"/>
+      <c r="S93" s="65"/>
+      <c r="T93" s="65"/>
+      <c r="U93" s="65"/>
+      <c r="V93" s="65"/>
+      <c r="W93" s="65"/>
+      <c r="X93" s="65"/>
+      <c r="Y93" s="65"/>
+      <c r="Z93" s="65"/>
+      <c r="AA93" s="65"/>
+      <c r="AB93" s="65"/>
     </row>
     <row r="94" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A94" s="21"/>
@@ -3562,50 +3562,50 @@
       <c r="M94" s="21"/>
       <c r="N94" s="21"/>
       <c r="O94" s="21"/>
-      <c r="P94" s="85" t="s">
+      <c r="P94" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="Q94" s="63"/>
-      <c r="R94" s="63"/>
-      <c r="S94" s="63"/>
-      <c r="T94" s="63"/>
-      <c r="U94" s="63"/>
-      <c r="V94" s="63"/>
-      <c r="W94" s="63"/>
-      <c r="X94" s="63"/>
-      <c r="Y94" s="63"/>
-      <c r="Z94" s="63"/>
-      <c r="AA94" s="63"/>
-      <c r="AB94" s="63"/>
+      <c r="Q94" s="57"/>
+      <c r="R94" s="57"/>
+      <c r="S94" s="57"/>
+      <c r="T94" s="57"/>
+      <c r="U94" s="57"/>
+      <c r="V94" s="57"/>
+      <c r="W94" s="57"/>
+      <c r="X94" s="57"/>
+      <c r="Y94" s="57"/>
+      <c r="Z94" s="57"/>
+      <c r="AA94" s="57"/>
+      <c r="AB94" s="57"/>
     </row>
     <row r="95" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H95" s="86">
+      <c r="H95" s="66">
         <f>B69</f>
         <v>0</v>
       </c>
-      <c r="I95" s="86"/>
-      <c r="J95" s="86"/>
-      <c r="K95" s="86"/>
-      <c r="L95" s="86"/>
-      <c r="M95" s="86"/>
-      <c r="N95" s="86"/>
-      <c r="O95" s="86"/>
-      <c r="P95" s="86"/>
-      <c r="Q95" s="86"/>
-      <c r="R95" s="86"/>
-      <c r="S95" s="86"/>
-      <c r="T95" s="86"/>
-      <c r="U95" s="86"/>
-      <c r="V95" s="86"/>
-      <c r="W95" s="86"/>
-      <c r="X95" s="86"/>
-      <c r="Y95" s="86"/>
-      <c r="Z95" s="86"/>
-      <c r="AA95" s="86"/>
-      <c r="AB95" s="86"/>
+      <c r="I95" s="66"/>
+      <c r="J95" s="66"/>
+      <c r="K95" s="66"/>
+      <c r="L95" s="66"/>
+      <c r="M95" s="66"/>
+      <c r="N95" s="66"/>
+      <c r="O95" s="66"/>
+      <c r="P95" s="66"/>
+      <c r="Q95" s="66"/>
+      <c r="R95" s="66"/>
+      <c r="S95" s="66"/>
+      <c r="T95" s="66"/>
+      <c r="U95" s="66"/>
+      <c r="V95" s="66"/>
+      <c r="W95" s="66"/>
+      <c r="X95" s="66"/>
+      <c r="Y95" s="66"/>
+      <c r="Z95" s="66"/>
+      <c r="AA95" s="66"/>
+      <c r="AB95" s="66"/>
     </row>
     <row r="96" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A96" s="21"/>
@@ -3616,52 +3616,52 @@
       <c r="F96" s="21"/>
       <c r="G96" s="21"/>
       <c r="H96" s="21"/>
-      <c r="I96" s="85" t="s">
+      <c r="I96" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="J96" s="63"/>
-      <c r="K96" s="63"/>
-      <c r="L96" s="63"/>
-      <c r="M96" s="63"/>
-      <c r="N96" s="63"/>
-      <c r="O96" s="63"/>
-      <c r="P96" s="63"/>
-      <c r="Q96" s="63"/>
-      <c r="R96" s="63"/>
-      <c r="S96" s="63"/>
-      <c r="T96" s="63"/>
-      <c r="U96" s="63"/>
-      <c r="V96" s="63"/>
-      <c r="W96" s="63"/>
-      <c r="X96" s="63"/>
-      <c r="Y96" s="63"/>
-      <c r="Z96" s="63"/>
-      <c r="AA96" s="63"/>
-      <c r="AB96" s="63"/>
+      <c r="J96" s="57"/>
+      <c r="K96" s="57"/>
+      <c r="L96" s="57"/>
+      <c r="M96" s="57"/>
+      <c r="N96" s="57"/>
+      <c r="O96" s="57"/>
+      <c r="P96" s="57"/>
+      <c r="Q96" s="57"/>
+      <c r="R96" s="57"/>
+      <c r="S96" s="57"/>
+      <c r="T96" s="57"/>
+      <c r="U96" s="57"/>
+      <c r="V96" s="57"/>
+      <c r="W96" s="57"/>
+      <c r="X96" s="57"/>
+      <c r="Y96" s="57"/>
+      <c r="Z96" s="57"/>
+      <c r="AA96" s="57"/>
+      <c r="AB96" s="57"/>
     </row>
     <row r="97" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J97" s="87"/>
-      <c r="K97" s="87"/>
-      <c r="L97" s="87"/>
-      <c r="M97" s="87"/>
-      <c r="N97" s="87"/>
-      <c r="O97" s="87"/>
-      <c r="P97" s="87"/>
-      <c r="Q97" s="87"/>
-      <c r="R97" s="87"/>
-      <c r="S97" s="87"/>
-      <c r="T97" s="87"/>
-      <c r="U97" s="87"/>
-      <c r="V97" s="87"/>
-      <c r="W97" s="87"/>
-      <c r="X97" s="87"/>
-      <c r="Y97" s="87"/>
-      <c r="Z97" s="87"/>
-      <c r="AA97" s="87"/>
-      <c r="AB97" s="87"/>
+      <c r="J97" s="56"/>
+      <c r="K97" s="56"/>
+      <c r="L97" s="56"/>
+      <c r="M97" s="56"/>
+      <c r="N97" s="56"/>
+      <c r="O97" s="56"/>
+      <c r="P97" s="56"/>
+      <c r="Q97" s="56"/>
+      <c r="R97" s="56"/>
+      <c r="S97" s="56"/>
+      <c r="T97" s="56"/>
+      <c r="U97" s="56"/>
+      <c r="V97" s="56"/>
+      <c r="W97" s="56"/>
+      <c r="X97" s="56"/>
+      <c r="Y97" s="56"/>
+      <c r="Z97" s="56"/>
+      <c r="AA97" s="56"/>
+      <c r="AB97" s="56"/>
     </row>
     <row r="98" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A98" s="21"/>
@@ -3674,47 +3674,47 @@
       <c r="H98" s="21"/>
       <c r="I98" s="21"/>
       <c r="J98" s="21"/>
-      <c r="K98" s="88" t="s">
+      <c r="K98" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="L98" s="63"/>
-      <c r="M98" s="63"/>
-      <c r="N98" s="63"/>
-      <c r="O98" s="63"/>
-      <c r="P98" s="63"/>
-      <c r="Q98" s="63"/>
-      <c r="R98" s="63"/>
-      <c r="S98" s="63"/>
-      <c r="T98" s="63"/>
-      <c r="U98" s="63"/>
-      <c r="V98" s="63"/>
-      <c r="W98" s="63"/>
-      <c r="X98" s="63"/>
-      <c r="Y98" s="63"/>
-      <c r="Z98" s="63"/>
-      <c r="AA98" s="63"/>
-      <c r="AB98" s="63"/>
+      <c r="L98" s="57"/>
+      <c r="M98" s="57"/>
+      <c r="N98" s="57"/>
+      <c r="O98" s="57"/>
+      <c r="P98" s="57"/>
+      <c r="Q98" s="57"/>
+      <c r="R98" s="57"/>
+      <c r="S98" s="57"/>
+      <c r="T98" s="57"/>
+      <c r="U98" s="57"/>
+      <c r="V98" s="57"/>
+      <c r="W98" s="57"/>
+      <c r="X98" s="57"/>
+      <c r="Y98" s="57"/>
+      <c r="Z98" s="57"/>
+      <c r="AA98" s="57"/>
+      <c r="AB98" s="57"/>
     </row>
     <row r="99" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="O99" s="67" t="s">
+      <c r="O99" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="P99" s="53"/>
-      <c r="Q99" s="53"/>
-      <c r="R99" s="53"/>
-      <c r="S99" s="53"/>
-      <c r="T99" s="53"/>
-      <c r="U99" s="53"/>
-      <c r="V99" s="53"/>
-      <c r="W99" s="53"/>
-      <c r="X99" s="53"/>
-      <c r="Y99" s="53"/>
-      <c r="Z99" s="53"/>
-      <c r="AA99" s="53"/>
-      <c r="AB99" s="53"/>
+      <c r="P99" s="60"/>
+      <c r="Q99" s="60"/>
+      <c r="R99" s="60"/>
+      <c r="S99" s="60"/>
+      <c r="T99" s="60"/>
+      <c r="U99" s="60"/>
+      <c r="V99" s="60"/>
+      <c r="W99" s="60"/>
+      <c r="X99" s="60"/>
+      <c r="Y99" s="60"/>
+      <c r="Z99" s="60"/>
+      <c r="AA99" s="60"/>
+      <c r="AB99" s="60"/>
     </row>
     <row r="100" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A100" s="41"/>
@@ -3731,22 +3731,22 @@
       <c r="L100" s="41"/>
       <c r="M100" s="41"/>
       <c r="N100" s="41"/>
-      <c r="O100" s="89" t="s">
+      <c r="O100" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="P100" s="50"/>
-      <c r="Q100" s="50"/>
-      <c r="R100" s="50"/>
-      <c r="S100" s="50"/>
-      <c r="T100" s="50"/>
-      <c r="U100" s="50"/>
-      <c r="V100" s="50"/>
-      <c r="W100" s="50"/>
-      <c r="X100" s="50"/>
-      <c r="Y100" s="50"/>
-      <c r="Z100" s="50"/>
-      <c r="AA100" s="50"/>
-      <c r="AB100" s="50"/>
+      <c r="P100" s="62"/>
+      <c r="Q100" s="62"/>
+      <c r="R100" s="62"/>
+      <c r="S100" s="62"/>
+      <c r="T100" s="62"/>
+      <c r="U100" s="62"/>
+      <c r="V100" s="62"/>
+      <c r="W100" s="62"/>
+      <c r="X100" s="62"/>
+      <c r="Y100" s="62"/>
+      <c r="Z100" s="62"/>
+      <c r="AA100" s="62"/>
+      <c r="AB100" s="62"/>
     </row>
     <row r="101" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
@@ -3779,26 +3779,26 @@
       <c r="C102" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L102" s="93">
+      <c r="L102" s="52">
         <f>M93</f>
         <v>0</v>
       </c>
-      <c r="M102" s="93"/>
-      <c r="N102" s="93"/>
-      <c r="O102" s="93"/>
-      <c r="P102" s="93"/>
-      <c r="Q102" s="93"/>
-      <c r="R102" s="93"/>
-      <c r="S102" s="93"/>
-      <c r="T102" s="93"/>
-      <c r="U102" s="93"/>
-      <c r="V102" s="93"/>
-      <c r="W102" s="93"/>
-      <c r="X102" s="93"/>
-      <c r="Y102" s="93"/>
-      <c r="Z102" s="93"/>
-      <c r="AA102" s="93"/>
-      <c r="AB102" s="93"/>
+      <c r="M102" s="52"/>
+      <c r="N102" s="52"/>
+      <c r="O102" s="52"/>
+      <c r="P102" s="52"/>
+      <c r="Q102" s="52"/>
+      <c r="R102" s="52"/>
+      <c r="S102" s="52"/>
+      <c r="T102" s="52"/>
+      <c r="U102" s="52"/>
+      <c r="V102" s="52"/>
+      <c r="W102" s="52"/>
+      <c r="X102" s="52"/>
+      <c r="Y102" s="52"/>
+      <c r="Z102" s="52"/>
+      <c r="AA102" s="52"/>
+      <c r="AB102" s="52"/>
     </row>
     <row r="103" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A103" s="21"/>
@@ -3813,24 +3813,24 @@
       <c r="J103" s="21"/>
       <c r="K103" s="21"/>
       <c r="L103" s="21"/>
-      <c r="M103" s="56" t="s">
+      <c r="M103" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="N103" s="57"/>
-      <c r="O103" s="57"/>
-      <c r="P103" s="57"/>
-      <c r="Q103" s="57"/>
-      <c r="R103" s="57"/>
-      <c r="S103" s="57"/>
-      <c r="T103" s="57"/>
-      <c r="U103" s="57"/>
-      <c r="V103" s="57"/>
-      <c r="W103" s="57"/>
-      <c r="X103" s="57"/>
-      <c r="Y103" s="57"/>
-      <c r="Z103" s="57"/>
-      <c r="AA103" s="57"/>
-      <c r="AB103" s="57"/>
+      <c r="N103" s="54"/>
+      <c r="O103" s="54"/>
+      <c r="P103" s="54"/>
+      <c r="Q103" s="54"/>
+      <c r="R103" s="54"/>
+      <c r="S103" s="54"/>
+      <c r="T103" s="54"/>
+      <c r="U103" s="54"/>
+      <c r="V103" s="54"/>
+      <c r="W103" s="54"/>
+      <c r="X103" s="54"/>
+      <c r="Y103" s="54"/>
+      <c r="Z103" s="54"/>
+      <c r="AA103" s="54"/>
+      <c r="AB103" s="54"/>
     </row>
     <row r="104" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
@@ -3873,94 +3873,94 @@
       <c r="J106" s="21"/>
       <c r="K106" s="21"/>
       <c r="L106" s="21"/>
-      <c r="M106" s="85" t="s">
+      <c r="M106" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="N106" s="85"/>
-      <c r="O106" s="85"/>
-      <c r="P106" s="85"/>
-      <c r="Q106" s="85"/>
-      <c r="R106" s="85"/>
-      <c r="S106" s="85"/>
-      <c r="T106" s="85"/>
-      <c r="U106" s="85"/>
-      <c r="V106" s="85"/>
-      <c r="W106" s="85"/>
-      <c r="X106" s="85"/>
-      <c r="Y106" s="85"/>
-      <c r="Z106" s="85"/>
-      <c r="AA106" s="85"/>
-      <c r="AB106" s="85"/>
+      <c r="N106" s="55"/>
+      <c r="O106" s="55"/>
+      <c r="P106" s="55"/>
+      <c r="Q106" s="55"/>
+      <c r="R106" s="55"/>
+      <c r="S106" s="55"/>
+      <c r="T106" s="55"/>
+      <c r="U106" s="55"/>
+      <c r="V106" s="55"/>
+      <c r="W106" s="55"/>
+      <c r="X106" s="55"/>
+      <c r="Y106" s="55"/>
+      <c r="Z106" s="55"/>
+      <c r="AA106" s="55"/>
+      <c r="AB106" s="55"/>
     </row>
     <row r="107" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A107" s="91" t="s">
+      <c r="A107" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="B107" s="91"/>
-      <c r="C107" s="91"/>
-      <c r="D107" s="91"/>
-      <c r="E107" s="91"/>
-      <c r="F107" s="91"/>
-      <c r="G107" s="91"/>
-      <c r="H107" s="91"/>
-      <c r="I107" s="91"/>
-      <c r="J107" s="91"/>
-      <c r="K107" s="91"/>
-      <c r="L107" s="91"/>
-      <c r="M107" s="91"/>
-      <c r="N107" s="91"/>
-      <c r="O107" s="91"/>
-      <c r="P107" s="91"/>
-      <c r="Q107" s="91"/>
-      <c r="R107" s="91"/>
-      <c r="S107" s="91"/>
-      <c r="T107" s="91"/>
-      <c r="U107" s="91"/>
-      <c r="V107" s="91"/>
-      <c r="W107" s="91"/>
-      <c r="X107" s="91"/>
-      <c r="Y107" s="91"/>
-      <c r="Z107" s="91"/>
-      <c r="AA107" s="91"/>
-      <c r="AB107" s="91"/>
+      <c r="B107" s="48"/>
+      <c r="C107" s="48"/>
+      <c r="D107" s="48"/>
+      <c r="E107" s="48"/>
+      <c r="F107" s="48"/>
+      <c r="G107" s="48"/>
+      <c r="H107" s="48"/>
+      <c r="I107" s="48"/>
+      <c r="J107" s="48"/>
+      <c r="K107" s="48"/>
+      <c r="L107" s="48"/>
+      <c r="M107" s="48"/>
+      <c r="N107" s="48"/>
+      <c r="O107" s="48"/>
+      <c r="P107" s="48"/>
+      <c r="Q107" s="48"/>
+      <c r="R107" s="48"/>
+      <c r="S107" s="48"/>
+      <c r="T107" s="48"/>
+      <c r="U107" s="48"/>
+      <c r="V107" s="48"/>
+      <c r="W107" s="48"/>
+      <c r="X107" s="48"/>
+      <c r="Y107" s="48"/>
+      <c r="Z107" s="48"/>
+      <c r="AA107" s="48"/>
+      <c r="AB107" s="48"/>
     </row>
     <row r="108" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H108" s="87"/>
-      <c r="I108" s="87"/>
-      <c r="J108" s="87"/>
-      <c r="K108" s="87"/>
-      <c r="L108" s="87"/>
-      <c r="M108" s="87"/>
-      <c r="N108" s="87"/>
-      <c r="O108" s="87"/>
-      <c r="P108" s="87"/>
-      <c r="Q108" s="87"/>
-      <c r="R108" s="87"/>
-      <c r="S108" s="87"/>
-      <c r="T108" s="87"/>
-      <c r="U108" s="87"/>
-      <c r="V108" s="87"/>
-      <c r="W108" s="87"/>
-      <c r="X108" s="87"/>
-      <c r="Y108" s="87"/>
-      <c r="Z108" s="87"/>
-      <c r="AA108" s="87"/>
-      <c r="AB108" s="87"/>
+      <c r="H108" s="56"/>
+      <c r="I108" s="56"/>
+      <c r="J108" s="56"/>
+      <c r="K108" s="56"/>
+      <c r="L108" s="56"/>
+      <c r="M108" s="56"/>
+      <c r="N108" s="56"/>
+      <c r="O108" s="56"/>
+      <c r="P108" s="56"/>
+      <c r="Q108" s="56"/>
+      <c r="R108" s="56"/>
+      <c r="S108" s="56"/>
+      <c r="T108" s="56"/>
+      <c r="U108" s="56"/>
+      <c r="V108" s="56"/>
+      <c r="W108" s="56"/>
+      <c r="X108" s="56"/>
+      <c r="Y108" s="56"/>
+      <c r="Z108" s="56"/>
+      <c r="AA108" s="56"/>
+      <c r="AB108" s="56"/>
     </row>
     <row r="109" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>56</v>
       </c>
       <c r="K109" s="45"/>
-      <c r="L109" s="52"/>
-      <c r="M109" s="52"/>
-      <c r="N109" s="52"/>
-      <c r="O109" s="52"/>
-      <c r="P109" s="52"/>
-      <c r="Q109" s="52"/>
+      <c r="L109" s="49"/>
+      <c r="M109" s="49"/>
+      <c r="N109" s="49"/>
+      <c r="O109" s="49"/>
+      <c r="P109" s="49"/>
+      <c r="Q109" s="49"/>
       <c r="R109" s="11"/>
       <c r="S109" s="17"/>
       <c r="T109" s="17"/>
@@ -3968,13 +3968,13 @@
       <c r="V109" s="17"/>
       <c r="W109" s="17"/>
       <c r="X109" s="11"/>
-      <c r="Y109" s="92">
+      <c r="Y109" s="50">
         <f>W67</f>
         <v>0</v>
       </c>
-      <c r="Z109" s="81"/>
-      <c r="AA109" s="81"/>
-      <c r="AB109" s="81"/>
+      <c r="Z109" s="51"/>
+      <c r="AA109" s="51"/>
+      <c r="AB109" s="51"/>
     </row>
     <row r="110" spans="1:28" x14ac:dyDescent="0.3">
       <c r="K110" s="11"/>
@@ -4010,12 +4010,12 @@
         <v>57</v>
       </c>
       <c r="K112" s="45"/>
-      <c r="L112" s="52"/>
-      <c r="M112" s="52"/>
-      <c r="N112" s="52"/>
-      <c r="O112" s="52"/>
-      <c r="P112" s="52"/>
-      <c r="Q112" s="52"/>
+      <c r="L112" s="49"/>
+      <c r="M112" s="49"/>
+      <c r="N112" s="49"/>
+      <c r="O112" s="49"/>
+      <c r="P112" s="49"/>
+      <c r="Q112" s="49"/>
       <c r="R112" s="11"/>
       <c r="S112" s="17"/>
       <c r="T112" s="17"/>
@@ -4023,13 +4023,13 @@
       <c r="V112" s="17"/>
       <c r="W112" s="17"/>
       <c r="X112" s="11"/>
-      <c r="Y112" s="92">
+      <c r="Y112" s="50">
         <f>W67</f>
         <v>0</v>
       </c>
-      <c r="Z112" s="81"/>
-      <c r="AA112" s="81"/>
-      <c r="AB112" s="81"/>
+      <c r="Z112" s="51"/>
+      <c r="AA112" s="51"/>
+      <c r="AB112" s="51"/>
     </row>
     <row r="113" spans="1:28" x14ac:dyDescent="0.3">
       <c r="K113" s="11"/>
@@ -4062,12 +4062,12 @@
         <v>52</v>
       </c>
       <c r="K114" s="45"/>
-      <c r="L114" s="52"/>
-      <c r="M114" s="52"/>
-      <c r="N114" s="52"/>
-      <c r="O114" s="52"/>
-      <c r="P114" s="52"/>
-      <c r="Q114" s="52"/>
+      <c r="L114" s="49"/>
+      <c r="M114" s="49"/>
+      <c r="N114" s="49"/>
+      <c r="O114" s="49"/>
+      <c r="P114" s="49"/>
+      <c r="Q114" s="49"/>
       <c r="R114" s="11"/>
       <c r="S114" s="17"/>
       <c r="T114" s="17"/>
@@ -4075,13 +4075,13 @@
       <c r="V114" s="17"/>
       <c r="W114" s="17"/>
       <c r="X114" s="11"/>
-      <c r="Y114" s="92">
+      <c r="Y114" s="50">
         <f>W67</f>
         <v>0</v>
       </c>
-      <c r="Z114" s="81"/>
-      <c r="AA114" s="81"/>
-      <c r="AB114" s="81"/>
+      <c r="Z114" s="51"/>
+      <c r="AA114" s="51"/>
+      <c r="AB114" s="51"/>
     </row>
     <row r="115" spans="1:28" x14ac:dyDescent="0.3">
       <c r="K115" s="11"/>
@@ -4114,12 +4114,12 @@
         <v>58</v>
       </c>
       <c r="K116" s="45"/>
-      <c r="L116" s="52"/>
-      <c r="M116" s="52"/>
-      <c r="N116" s="52"/>
-      <c r="O116" s="52"/>
-      <c r="P116" s="52"/>
-      <c r="Q116" s="52"/>
+      <c r="L116" s="49"/>
+      <c r="M116" s="49"/>
+      <c r="N116" s="49"/>
+      <c r="O116" s="49"/>
+      <c r="P116" s="49"/>
+      <c r="Q116" s="49"/>
       <c r="R116" s="11"/>
       <c r="S116" s="17"/>
       <c r="T116" s="17"/>
@@ -4127,13 +4127,13 @@
       <c r="V116" s="17"/>
       <c r="W116" s="17"/>
       <c r="X116" s="11"/>
-      <c r="Y116" s="92">
+      <c r="Y116" s="50">
         <f>W67</f>
         <v>0</v>
       </c>
-      <c r="Z116" s="81"/>
-      <c r="AA116" s="81"/>
-      <c r="AB116" s="81"/>
+      <c r="Z116" s="51"/>
+      <c r="AA116" s="51"/>
+      <c r="AB116" s="51"/>
     </row>
     <row r="117" spans="1:28" x14ac:dyDescent="0.3">
       <c r="K117" s="11"/>
@@ -4183,6 +4183,70 @@
     </row>
   </sheetData>
   <mergeCells count="80">
+    <mergeCell ref="A30:AB30"/>
+    <mergeCell ref="A31:AB31"/>
+    <mergeCell ref="J32:AB32"/>
+    <mergeCell ref="L57:Q57"/>
+    <mergeCell ref="Y57:AB57"/>
+    <mergeCell ref="A35:AB35"/>
+    <mergeCell ref="L51:Q51"/>
+    <mergeCell ref="Y51:AB51"/>
+    <mergeCell ref="L55:Q55"/>
+    <mergeCell ref="Y55:AB55"/>
+    <mergeCell ref="L53:Q53"/>
+    <mergeCell ref="Y53:AB53"/>
+    <mergeCell ref="A23:AB23"/>
+    <mergeCell ref="A25:AB25"/>
+    <mergeCell ref="I26:AB26"/>
+    <mergeCell ref="K27:AB27"/>
+    <mergeCell ref="M28:AB28"/>
+    <mergeCell ref="A1:AB1"/>
+    <mergeCell ref="E59:K59"/>
+    <mergeCell ref="F60:K60"/>
+    <mergeCell ref="T60:AB60"/>
+    <mergeCell ref="G61:K61"/>
+    <mergeCell ref="P61:S61"/>
+    <mergeCell ref="T61:AB63"/>
+    <mergeCell ref="D62:K62"/>
+    <mergeCell ref="I20:AB20"/>
+    <mergeCell ref="A3:AB4"/>
+    <mergeCell ref="A8:AB9"/>
+    <mergeCell ref="I14:AB14"/>
+    <mergeCell ref="I16:AB16"/>
+    <mergeCell ref="I18:AB18"/>
+    <mergeCell ref="G21:P21"/>
+    <mergeCell ref="G22:P22"/>
+    <mergeCell ref="R64:S64"/>
+    <mergeCell ref="T64:AB64"/>
+    <mergeCell ref="T65:AB65"/>
+    <mergeCell ref="Q66:AB66"/>
+    <mergeCell ref="M67:O67"/>
+    <mergeCell ref="W67:AB67"/>
+    <mergeCell ref="A68:AB68"/>
+    <mergeCell ref="B69:AA69"/>
+    <mergeCell ref="A70:AB70"/>
+    <mergeCell ref="I73:AB73"/>
+    <mergeCell ref="I75:AB75"/>
+    <mergeCell ref="I77:AB77"/>
+    <mergeCell ref="I79:AB79"/>
+    <mergeCell ref="I81:AB81"/>
+    <mergeCell ref="G82:P82"/>
+    <mergeCell ref="G83:P83"/>
+    <mergeCell ref="A84:AB84"/>
+    <mergeCell ref="A86:AB86"/>
+    <mergeCell ref="I87:AB87"/>
+    <mergeCell ref="K88:AB88"/>
+    <mergeCell ref="M89:AB89"/>
+    <mergeCell ref="A91:AB91"/>
+    <mergeCell ref="A92:AB92"/>
+    <mergeCell ref="M93:AB93"/>
+    <mergeCell ref="P94:AB94"/>
+    <mergeCell ref="H95:AB95"/>
+    <mergeCell ref="I96:AB96"/>
+    <mergeCell ref="J97:AB97"/>
+    <mergeCell ref="K98:AB98"/>
+    <mergeCell ref="O99:AB99"/>
+    <mergeCell ref="O100:AB100"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="A55:K55"/>
     <mergeCell ref="A57:K57"/>
@@ -4199,70 +4263,6 @@
     <mergeCell ref="M106:AB106"/>
     <mergeCell ref="A107:AB107"/>
     <mergeCell ref="H108:AB108"/>
-    <mergeCell ref="I96:AB96"/>
-    <mergeCell ref="J97:AB97"/>
-    <mergeCell ref="K98:AB98"/>
-    <mergeCell ref="O99:AB99"/>
-    <mergeCell ref="O100:AB100"/>
-    <mergeCell ref="A91:AB91"/>
-    <mergeCell ref="A92:AB92"/>
-    <mergeCell ref="M93:AB93"/>
-    <mergeCell ref="P94:AB94"/>
-    <mergeCell ref="H95:AB95"/>
-    <mergeCell ref="A84:AB84"/>
-    <mergeCell ref="A86:AB86"/>
-    <mergeCell ref="I87:AB87"/>
-    <mergeCell ref="K88:AB88"/>
-    <mergeCell ref="M89:AB89"/>
-    <mergeCell ref="I77:AB77"/>
-    <mergeCell ref="I79:AB79"/>
-    <mergeCell ref="I81:AB81"/>
-    <mergeCell ref="G82:P82"/>
-    <mergeCell ref="G83:P83"/>
-    <mergeCell ref="A68:AB68"/>
-    <mergeCell ref="B69:AA69"/>
-    <mergeCell ref="A70:AB70"/>
-    <mergeCell ref="I73:AB73"/>
-    <mergeCell ref="I75:AB75"/>
-    <mergeCell ref="R64:S64"/>
-    <mergeCell ref="T64:AB64"/>
-    <mergeCell ref="T65:AB65"/>
-    <mergeCell ref="Q66:AB66"/>
-    <mergeCell ref="M67:O67"/>
-    <mergeCell ref="W67:AB67"/>
-    <mergeCell ref="A1:AB1"/>
-    <mergeCell ref="E59:K59"/>
-    <mergeCell ref="F60:K60"/>
-    <mergeCell ref="T60:AB60"/>
-    <mergeCell ref="G61:K61"/>
-    <mergeCell ref="P61:S61"/>
-    <mergeCell ref="T61:AB63"/>
-    <mergeCell ref="D62:K62"/>
-    <mergeCell ref="I20:AB20"/>
-    <mergeCell ref="A3:AB4"/>
-    <mergeCell ref="A8:AB9"/>
-    <mergeCell ref="I14:AB14"/>
-    <mergeCell ref="I16:AB16"/>
-    <mergeCell ref="I18:AB18"/>
-    <mergeCell ref="G21:P21"/>
-    <mergeCell ref="G22:P22"/>
-    <mergeCell ref="A23:AB23"/>
-    <mergeCell ref="A25:AB25"/>
-    <mergeCell ref="I26:AB26"/>
-    <mergeCell ref="K27:AB27"/>
-    <mergeCell ref="M28:AB28"/>
-    <mergeCell ref="A30:AB30"/>
-    <mergeCell ref="A31:AB31"/>
-    <mergeCell ref="J32:AB32"/>
-    <mergeCell ref="L57:Q57"/>
-    <mergeCell ref="Y57:AB57"/>
-    <mergeCell ref="A35:AB35"/>
-    <mergeCell ref="L51:Q51"/>
-    <mergeCell ref="Y51:AB51"/>
-    <mergeCell ref="L55:Q55"/>
-    <mergeCell ref="Y55:AB55"/>
-    <mergeCell ref="L53:Q53"/>
-    <mergeCell ref="Y53:AB53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="93" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>